<commit_message>
More Fixes to localisation implementation
</commit_message>
<xml_diff>
--- a/suppxls/Scen_Localisation-Hi.xlsx
+++ b/suppxls/Scen_Localisation-Hi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{706CA360-827E-439D-A5C8-B88FACDB3806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E8D8D32-14B9-4278-8754-C8DE62A6F923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="15" windowWidth="28770" windowHeight="15570" xr2:uid="{232E471A-D1BC-46EA-822F-4A9C8F9BFC34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{232E471A-D1BC-46EA-822F-4A9C8F9BFC34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={BFF637BF-F295-4BD2-8A3C-4C0D24997E80}</author>
+  </authors>
+  <commentList>
+    <comment ref="U24" authorId="0" shapeId="0" xr:uid="{BFF637BF-F295-4BD2-8A3C-4C0D24997E80}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    This must be re-activated when Reference costs are changed. One must leave it de-activated for High Localisation scenarios</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="136">
   <si>
     <t>~TFM_INS-TS</t>
   </si>
@@ -353,9 +371,6 @@
     <t>XUPSELC</t>
   </si>
   <si>
-    <t>~TFM_FILL</t>
-  </si>
-  <si>
     <t>Update values</t>
   </si>
   <si>
@@ -444,6 +459,9 @@
   </si>
   <si>
     <t>Cost Increase</t>
+  </si>
+  <si>
+    <t>TFM_FILL</t>
   </si>
 </sst>
 </file>
@@ -779,6 +797,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Bruno Merven" id="{B5E69722-C63D-4CBF-877A-AF5854BD44E9}" userId="S::01405439@wf.uct.ac.za::c7f06137-2c3b-4c5c-8f38-fe1abbc96860" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1074,11 +1098,19 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="U24" dT="2023-12-19T09:22:03.61" personId="{B5E69722-C63D-4CBF-877A-AF5854BD44E9}" id="{BFF637BF-F295-4BD2-8A3C-4C0D24997E80}">
+    <text>This must be re-activated when Reference costs are changed. One must leave it de-activated for High Localisation scenarios</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C1C3BE-43A3-4F6E-B7BA-55F1C4F1EF02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C1C3BE-43A3-4F6E-B7BA-55F1C4F1EF02}">
   <dimension ref="B2:BL83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1093,17 +1125,17 @@
   <sheetData>
     <row r="2" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C2" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C3" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E4" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="3:14" x14ac:dyDescent="0.25">
@@ -1131,7 +1163,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G6" s="4">
         <f>1-M32</f>
@@ -1163,7 +1195,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G7" s="4">
         <f>1-L32</f>
@@ -1192,10 +1224,10 @@
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G8" s="4">
         <f>1-N32</f>
@@ -1224,10 +1256,10 @@
     </row>
     <row r="9" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G9" s="4">
         <f>1-O32</f>
@@ -1256,7 +1288,7 @@
     </row>
     <row r="12" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C12" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="3:14" x14ac:dyDescent="0.25">
@@ -1382,13 +1414,13 @@
     </row>
     <row r="18" spans="3:64" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D18" t="s">
         <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F18" t="s">
         <v>19</v>
@@ -1418,7 +1450,7 @@
         <v>0.21901639344262303</v>
       </c>
       <c r="T18" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U18" s="13"/>
       <c r="V18" s="13"/>
@@ -1467,13 +1499,13 @@
     </row>
     <row r="19" spans="3:64" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F19" t="s">
         <v>19</v>
@@ -1503,20 +1535,20 @@
         <v>5.1724137931034475E-2</v>
       </c>
       <c r="T19" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21" spans="3:64" x14ac:dyDescent="0.25">
       <c r="AZ21" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="3:64" x14ac:dyDescent="0.25">
       <c r="T22" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AZ22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="BB22" s="4">
         <f>SUMIF($F$66:$F$69,$C$3,G66:G69)</f>
@@ -1547,29 +1579,34 @@
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="3:64" x14ac:dyDescent="0.25">
-      <c r="U24" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z24" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE24" t="s">
-        <v>105</v>
-      </c>
-      <c r="AJ24" t="s">
-        <v>105</v>
-      </c>
-      <c r="AP24" t="s">
-        <v>105</v>
-      </c>
-      <c r="AU24" t="s">
-        <v>105</v>
+      <c r="U24" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="Z24" t="str">
+        <f>U24</f>
+        <v>TFM_FILL</v>
+      </c>
+      <c r="AE24" t="str">
+        <f>Z24</f>
+        <v>TFM_FILL</v>
+      </c>
+      <c r="AJ24" t="str">
+        <f>AE24</f>
+        <v>TFM_FILL</v>
+      </c>
+      <c r="AP24" t="str">
+        <f>AJ24</f>
+        <v>TFM_FILL</v>
+      </c>
+      <c r="AU24" t="str">
+        <f>AP24</f>
+        <v>TFM_FILL</v>
       </c>
       <c r="AZ24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="BJ24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="3:64" x14ac:dyDescent="0.25">
@@ -1898,7 +1935,7 @@
         <v>2017</v>
       </c>
       <c r="X28">
-        <v>60837.512560000003</v>
+        <v>55306.829599999997</v>
       </c>
       <c r="Z28" s="7" t="s">
         <v>21</v>
@@ -1960,7 +1997,7 @@
       </c>
       <c r="BB28">
         <f t="shared" si="10"/>
-        <v>60837.512560000003</v>
+        <v>55306.829599999997</v>
       </c>
       <c r="BC28" t="str">
         <f t="shared" si="11"/>
@@ -2021,7 +2058,7 @@
         <v>2017</v>
       </c>
       <c r="X29">
-        <v>117681.09583999999</v>
+        <v>106982.8144</v>
       </c>
       <c r="Z29" s="7" t="s">
         <v>21</v>
@@ -2083,7 +2120,7 @@
       </c>
       <c r="BB29">
         <f t="shared" si="10"/>
-        <v>117681.09583999999</v>
+        <v>106982.8144</v>
       </c>
       <c r="BC29" t="str">
         <f t="shared" si="11"/>
@@ -2149,7 +2186,7 @@
         <v>2017</v>
       </c>
       <c r="X30">
-        <v>34722.7166</v>
+        <v>31566.106</v>
       </c>
       <c r="Z30" s="7" t="s">
         <v>21</v>
@@ -2211,7 +2248,7 @@
       </c>
       <c r="BB30">
         <f t="shared" si="10"/>
-        <v>34722.7166</v>
+        <v>31566.106</v>
       </c>
       <c r="BC30" t="str">
         <f t="shared" si="11"/>
@@ -2270,10 +2307,10 @@
         <v>cmach_e</v>
       </c>
       <c r="N31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="O31" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="T31" s="9" t="s">
         <v>35</v>
@@ -2288,7 +2325,7 @@
         <v>2017</v>
       </c>
       <c r="X31">
-        <v>73433.283439999999</v>
+        <v>66757.530400000003</v>
       </c>
       <c r="Z31" s="7" t="s">
         <v>21</v>
@@ -2350,7 +2387,7 @@
       </c>
       <c r="BB31">
         <f t="shared" si="10"/>
-        <v>73433.283439999999</v>
+        <v>66757.530400000003</v>
       </c>
       <c r="BC31" t="str">
         <f t="shared" si="11"/>
@@ -2429,7 +2466,7 @@
         <v>2017</v>
       </c>
       <c r="X32">
-        <v>106024.612628</v>
+        <v>96386.011480000001</v>
       </c>
       <c r="Z32" s="7" t="s">
         <v>21</v>
@@ -2491,7 +2528,7 @@
       </c>
       <c r="BB32">
         <f t="shared" si="10"/>
-        <v>106024.612628</v>
+        <v>96386.011480000001</v>
       </c>
       <c r="BC32" t="str">
         <f t="shared" si="11"/>
@@ -2547,7 +2584,7 @@
         <v>2017</v>
       </c>
       <c r="X33">
-        <v>89407.982771283598</v>
+        <v>81279.984337530506</v>
       </c>
       <c r="Z33" s="7" t="s">
         <v>21</v>
@@ -2560,7 +2597,7 @@
         <v>2020</v>
       </c>
       <c r="AC33">
-        <v>81398.386302773797</v>
+        <v>73998.533002521595</v>
       </c>
       <c r="AE33" s="7" t="s">
         <v>21</v>
@@ -2573,7 +2610,7 @@
         <v>2025</v>
       </c>
       <c r="AH33">
-        <v>68049.058855257405</v>
+        <v>61862.780777506698</v>
       </c>
       <c r="AJ33" s="7" t="s">
         <v>21</v>
@@ -2586,7 +2623,7 @@
         <v>2030</v>
       </c>
       <c r="AM33">
-        <v>54699.731407741099</v>
+        <v>49727.028552491902</v>
       </c>
       <c r="AP33" s="7" t="s">
         <v>21</v>
@@ -2599,7 +2636,7 @@
         <v>2040</v>
       </c>
       <c r="AS33">
-        <v>54699.731407741099</v>
+        <v>49727.028552491902</v>
       </c>
       <c r="AU33" s="7" t="s">
         <v>21</v>
@@ -2612,7 +2649,7 @@
         <v>2050</v>
       </c>
       <c r="AX33">
-        <v>54699.731407741099</v>
+        <v>49727.028552491902</v>
       </c>
       <c r="AZ33" t="str">
         <f t="shared" si="20"/>
@@ -2624,27 +2661,27 @@
       </c>
       <c r="BB33">
         <f t="shared" si="10"/>
-        <v>89407.982771283598</v>
+        <v>81279.984337530506</v>
       </c>
       <c r="BC33">
         <f t="shared" si="11"/>
-        <v>81398.386302773797</v>
+        <v>73998.533002521595</v>
       </c>
       <c r="BD33">
         <f t="shared" si="12"/>
-        <v>69410.040032362551</v>
+        <v>63100.036393056835</v>
       </c>
       <c r="BE33">
         <f t="shared" si="13"/>
-        <v>57434.717978128159</v>
+        <v>52213.379980116501</v>
       </c>
       <c r="BF33">
         <f t="shared" si="14"/>
-        <v>58802.211263321682</v>
+        <v>53456.555693928793</v>
       </c>
       <c r="BG33">
         <f t="shared" si="15"/>
-        <v>60169.704548515212</v>
+        <v>54699.731407741099</v>
       </c>
       <c r="BJ33">
         <v>1</v>
@@ -2677,7 +2714,7 @@
         <v>2017</v>
       </c>
       <c r="X34">
-        <v>21455.514407079601</v>
+        <v>19505.013097345101</v>
       </c>
       <c r="Z34" s="7" t="s">
         <v>21</v>
@@ -2690,7 +2727,7 @@
         <v>2020</v>
       </c>
       <c r="AC34">
-        <v>15191.2526690265</v>
+        <v>13810.229699115</v>
       </c>
       <c r="AE34" s="7" t="s">
         <v>21</v>
@@ -2703,7 +2740,7 @@
         <v>2025</v>
       </c>
       <c r="AH34">
-        <v>14259.843614159299</v>
+        <v>12963.4941946903</v>
       </c>
       <c r="AJ34" s="7" t="s">
         <v>21</v>
@@ -2716,7 +2753,7 @@
         <v>2030</v>
       </c>
       <c r="AM34">
-        <v>13396.6218265486</v>
+        <v>12178.7471150442</v>
       </c>
       <c r="AP34" s="7" t="s">
         <v>21</v>
@@ -2729,7 +2766,7 @@
         <v>2040</v>
       </c>
       <c r="AS34">
-        <v>11900.8543256637</v>
+        <v>10818.9584778761</v>
       </c>
       <c r="AU34" s="7" t="s">
         <v>21</v>
@@ -2742,7 +2779,7 @@
         <v>2050</v>
       </c>
       <c r="AX34">
-        <v>10513.896293805299</v>
+        <v>9558.0875398230091</v>
       </c>
       <c r="AZ34" t="str">
         <f t="shared" si="20"/>
@@ -2754,27 +2791,27 @@
       </c>
       <c r="BB34">
         <f t="shared" si="10"/>
-        <v>21455.514407079601</v>
+        <v>19505.013097345101</v>
       </c>
       <c r="BC34">
         <f t="shared" si="11"/>
-        <v>15191.2526690265</v>
+        <v>13810.229699115</v>
       </c>
       <c r="BD34">
         <f t="shared" si="12"/>
-        <v>14545.040486442485</v>
+        <v>13222.764078584107</v>
       </c>
       <c r="BE34">
         <f t="shared" si="13"/>
-        <v>14066.452917876031</v>
+        <v>12787.68447079641</v>
       </c>
       <c r="BF34">
         <f t="shared" si="14"/>
-        <v>12793.418400088478</v>
+        <v>11630.380363716808</v>
       </c>
       <c r="BG34">
         <f t="shared" si="15"/>
-        <v>11565.285923185829</v>
+        <v>10513.89629380531</v>
       </c>
       <c r="BJ34">
         <v>1</v>
@@ -2794,7 +2831,7 @@
         <v>2017</v>
       </c>
       <c r="X35">
-        <v>22872.387999999999</v>
+        <v>20793.080000000002</v>
       </c>
       <c r="Z35" s="7" t="s">
         <v>21</v>
@@ -2807,7 +2844,7 @@
         <v>2020</v>
       </c>
       <c r="AC35">
-        <v>16194.4486</v>
+        <v>14722.226000000001</v>
       </c>
       <c r="AE35" s="7" t="s">
         <v>21</v>
@@ -2820,7 +2857,7 @@
         <v>2025</v>
       </c>
       <c r="AH35">
-        <v>15201.5314</v>
+        <v>13819.574000000001</v>
       </c>
       <c r="AJ35" s="7" t="s">
         <v>21</v>
@@ -2833,7 +2870,7 @@
         <v>2030</v>
       </c>
       <c r="AM35">
-        <v>14281.304400000001</v>
+        <v>12983.004000000001</v>
       </c>
       <c r="AP35" s="7" t="s">
         <v>21</v>
@@ -2846,7 +2883,7 @@
         <v>2040</v>
       </c>
       <c r="AS35">
-        <v>12686.7598</v>
+        <v>11533.418</v>
       </c>
       <c r="AU35" s="7" t="s">
         <v>21</v>
@@ -2859,7 +2896,7 @@
         <v>2050</v>
       </c>
       <c r="AX35">
-        <v>11208.2102</v>
+        <v>10189.281999999999</v>
       </c>
       <c r="AZ35" t="str">
         <f t="shared" si="20"/>
@@ -2871,27 +2908,27 @@
       </c>
       <c r="BB35">
         <f t="shared" si="10"/>
-        <v>22872.387999999999</v>
+        <v>20793.080000000002</v>
       </c>
       <c r="BC35">
         <f t="shared" si="11"/>
-        <v>16194.4486</v>
+        <v>14722.226000000001</v>
       </c>
       <c r="BD35">
         <f t="shared" si="12"/>
-        <v>15505.562028</v>
+        <v>14095.965480000001</v>
       </c>
       <c r="BE35">
         <f t="shared" si="13"/>
-        <v>14995.369620000001</v>
+        <v>13632.154200000001</v>
       </c>
       <c r="BF35">
         <f t="shared" si="14"/>
-        <v>13638.266785</v>
+        <v>12398.424349999999</v>
       </c>
       <c r="BG35">
         <f t="shared" si="15"/>
-        <v>12329.031220000001</v>
+        <v>11208.2102</v>
       </c>
       <c r="BJ35">
         <v>1</v>
@@ -2911,7 +2948,7 @@
         <v>2017</v>
       </c>
       <c r="X36">
-        <v>23683.387200000001</v>
+        <v>21530.351999999999</v>
       </c>
       <c r="Z36" s="7" t="s">
         <v>21</v>
@@ -2924,7 +2961,7 @@
         <v>2020</v>
       </c>
       <c r="AC36">
-        <v>19332.5</v>
+        <v>17575</v>
       </c>
       <c r="AE36" s="7" t="s">
         <v>21</v>
@@ -2937,7 +2974,7 @@
         <v>2025</v>
       </c>
       <c r="AH36">
-        <v>19163.920600000001</v>
+        <v>17421.745999999999</v>
       </c>
       <c r="AJ36" s="7" t="s">
         <v>21</v>
@@ -2950,7 +2987,7 @@
         <v>2030</v>
       </c>
       <c r="AM36">
-        <v>18996.8878</v>
+        <v>17269.898000000001</v>
       </c>
       <c r="AP36" s="7" t="s">
         <v>21</v>
@@ -2963,7 +3000,7 @@
         <v>2040</v>
       </c>
       <c r="AS36">
-        <v>18665.915400000002</v>
+        <v>16969.013999999999</v>
       </c>
       <c r="AU36" s="7" t="s">
         <v>21</v>
@@ -2976,7 +3013,7 @@
         <v>2050</v>
       </c>
       <c r="AX36">
-        <v>18341.129400000002</v>
+        <v>16673.754000000001</v>
       </c>
       <c r="AZ36" t="str">
         <f t="shared" si="20"/>
@@ -2988,27 +3025,27 @@
       </c>
       <c r="BB36">
         <f t="shared" si="10"/>
-        <v>23683.387200000001</v>
+        <v>21530.351999999999</v>
       </c>
       <c r="BC36">
         <f t="shared" si="11"/>
-        <v>19332.5</v>
+        <v>17575</v>
       </c>
       <c r="BD36">
         <f t="shared" si="12"/>
-        <v>19547.199012000001</v>
+        <v>17770.180919999999</v>
       </c>
       <c r="BE36">
         <f t="shared" si="13"/>
-        <v>19946.732190000002</v>
+        <v>18133.392900000003</v>
       </c>
       <c r="BF36">
         <f t="shared" si="14"/>
-        <v>20065.859055000001</v>
+        <v>18241.690049999997</v>
       </c>
       <c r="BG36">
         <f t="shared" si="15"/>
-        <v>20175.242340000004</v>
+        <v>18341.129400000002</v>
       </c>
       <c r="BJ36">
         <v>1</v>
@@ -3028,7 +3065,7 @@
         <v>2017</v>
       </c>
       <c r="X37">
-        <v>14021.305759999999</v>
+        <v>12746.641600000001</v>
       </c>
       <c r="Z37" s="7" t="s">
         <v>21</v>
@@ -3090,7 +3127,7 @@
       </c>
       <c r="BB37">
         <f t="shared" si="10"/>
-        <v>14021.305759999999</v>
+        <v>12746.641600000001</v>
       </c>
       <c r="BC37" t="str">
         <f t="shared" si="11"/>
@@ -3118,7 +3155,7 @@
     </row>
     <row r="38" spans="2:62" x14ac:dyDescent="0.25">
       <c r="B38" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T38" s="9" t="s">
         <v>49</v>
@@ -3133,7 +3170,7 @@
         <v>2017</v>
       </c>
       <c r="X38">
-        <v>38234.504000000001</v>
+        <v>34758.639999999999</v>
       </c>
       <c r="Z38" s="7" t="s">
         <v>21</v>
@@ -3195,7 +3232,7 @@
       </c>
       <c r="BB38">
         <f t="shared" si="10"/>
-        <v>38234.504000000001</v>
+        <v>34758.639999999999</v>
       </c>
       <c r="BC38" t="str">
         <f t="shared" si="11"/>
@@ -3235,7 +3272,7 @@
         <v>2017</v>
       </c>
       <c r="X39">
-        <v>15396.688560000001</v>
+        <v>13996.989600000001</v>
       </c>
       <c r="Z39" s="7" t="s">
         <v>21</v>
@@ -3297,7 +3334,7 @@
       </c>
       <c r="BB39">
         <f t="shared" si="10"/>
-        <v>15396.688560000001</v>
+        <v>13996.989600000001</v>
       </c>
       <c r="BC39" t="str">
         <f t="shared" si="11"/>
@@ -3325,7 +3362,7 @@
     </row>
     <row r="40" spans="2:62" x14ac:dyDescent="0.25">
       <c r="C40" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G40" s="2">
         <v>2017</v>
@@ -3358,7 +3395,7 @@
         <v>2017</v>
       </c>
       <c r="X40">
-        <v>33832.897120000001</v>
+        <v>30757.179199999999</v>
       </c>
       <c r="Z40" s="7" t="s">
         <v>21</v>
@@ -3420,7 +3457,7 @@
       </c>
       <c r="BB40">
         <f t="shared" si="10"/>
-        <v>33832.897120000001</v>
+        <v>30757.179199999999</v>
       </c>
       <c r="BC40" t="str">
         <f t="shared" si="11"/>
@@ -3451,7 +3488,7 @@
         <v>8</v>
       </c>
       <c r="F41" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G41" s="5">
         <f>1-M32</f>
@@ -3486,7 +3523,7 @@
         <v>2017</v>
       </c>
       <c r="X41">
-        <v>21875.425439999999</v>
+        <v>19886.750400000001</v>
       </c>
       <c r="Z41" s="7" t="s">
         <v>21</v>
@@ -3548,7 +3585,7 @@
       </c>
       <c r="BB41">
         <f t="shared" si="10"/>
-        <v>21875.425439999999</v>
+        <v>19886.750400000001</v>
       </c>
       <c r="BC41" t="str">
         <f t="shared" si="11"/>
@@ -3580,7 +3617,7 @@
         <v>cmach_e</v>
       </c>
       <c r="F42" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G42" s="5">
         <f>G41</f>
@@ -3615,7 +3652,7 @@
         <v>2017</v>
       </c>
       <c r="X42">
-        <v>29248.437984222699</v>
+        <v>26589.4890765661</v>
       </c>
       <c r="Z42" s="7" t="s">
         <v>21</v>
@@ -3677,7 +3714,7 @@
       </c>
       <c r="BB42">
         <f t="shared" si="10"/>
-        <v>29248.437984222699</v>
+        <v>26589.4890765661</v>
       </c>
       <c r="BC42" t="str">
         <f t="shared" si="11"/>
@@ -3709,7 +3746,7 @@
         <v>cmach_e</v>
       </c>
       <c r="F43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G43" s="5">
         <f>G42</f>
@@ -3744,7 +3781,7 @@
         <v>2017</v>
       </c>
       <c r="X43">
-        <v>29248.437984222699</v>
+        <v>26589.4890765661</v>
       </c>
       <c r="Z43" s="7" t="s">
         <v>21</v>
@@ -3806,7 +3843,7 @@
       </c>
       <c r="BB43">
         <f t="shared" si="10"/>
-        <v>29248.437984222699</v>
+        <v>26589.4890765661</v>
       </c>
       <c r="BC43" t="str">
         <f t="shared" si="11"/>
@@ -3838,7 +3875,7 @@
         <v>cmach_e</v>
       </c>
       <c r="F44" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G44" s="5">
         <f>G43</f>
@@ -3865,7 +3902,7 @@
         <v>0.47058823529411764</v>
       </c>
       <c r="N44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T44" s="9" t="s">
         <v>61</v>
@@ -3880,7 +3917,7 @@
         <v>2017</v>
       </c>
       <c r="X44">
-        <v>42015.284959999997</v>
+        <v>38195.713600000003</v>
       </c>
       <c r="Z44" s="7" t="s">
         <v>21</v>
@@ -3893,7 +3930,7 @@
         <v>2020</v>
       </c>
       <c r="AC44">
-        <v>26933.083740014099</v>
+        <v>24484.621581831001</v>
       </c>
       <c r="AE44" s="7" t="s">
         <v>21</v>
@@ -3906,7 +3943,7 @@
         <v>2025</v>
       </c>
       <c r="AH44">
-        <v>26591.811125704</v>
+        <v>24174.373750639999</v>
       </c>
       <c r="AJ44" s="7" t="s">
         <v>21</v>
@@ -3919,7 +3956,7 @@
         <v>2030</v>
       </c>
       <c r="AM44">
-        <v>22290.023759944099</v>
+        <v>20263.657963585501</v>
       </c>
       <c r="AP44" s="7" t="s">
         <v>21</v>
@@ -3932,7 +3969,7 @@
         <v>2040</v>
       </c>
       <c r="AS44">
-        <v>18852.7362232987</v>
+        <v>17138.851112089698</v>
       </c>
       <c r="AU44" s="7" t="s">
         <v>21</v>
@@ -3945,7 +3982,7 @@
         <v>2050</v>
       </c>
       <c r="AX44">
-        <v>15417.019777003599</v>
+        <v>14015.472524548701</v>
       </c>
       <c r="AZ44" t="str">
         <f t="shared" si="20"/>
@@ -3957,27 +3994,27 @@
       </c>
       <c r="BB44">
         <f t="shared" si="10"/>
-        <v>42015.284959999997</v>
+        <v>38195.713600000003</v>
       </c>
       <c r="BC44">
         <f t="shared" si="11"/>
-        <v>26933.083740014099</v>
+        <v>24484.621581831001</v>
       </c>
       <c r="BD44">
         <f t="shared" si="12"/>
-        <v>27123.647348218081</v>
+        <v>24657.861225652799</v>
       </c>
       <c r="BE44">
         <f t="shared" si="13"/>
-        <v>23404.524947941303</v>
+        <v>21276.840861764776</v>
       </c>
       <c r="BF44">
         <f t="shared" si="14"/>
-        <v>20266.691440046103</v>
+        <v>18424.264945496427</v>
       </c>
       <c r="BG44">
         <f t="shared" si="15"/>
-        <v>16958.721754703962</v>
+        <v>15417.019777003572</v>
       </c>
       <c r="BJ44">
         <v>1</v>
@@ -3997,7 +4034,7 @@
         <v>2017</v>
       </c>
       <c r="X45">
-        <v>24888.396712212401</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="Z45" s="7" t="s">
         <v>21</v>
@@ -4010,7 +4047,7 @@
         <v>2020</v>
       </c>
       <c r="AC45">
-        <v>17621.853096070899</v>
+        <v>16019.866450973501</v>
       </c>
       <c r="AE45" s="7" t="s">
         <v>21</v>
@@ -4023,7 +4060,7 @@
         <v>2025</v>
       </c>
       <c r="AH45">
-        <v>16541.418592424801</v>
+        <v>15037.6532658407</v>
       </c>
       <c r="AJ45" s="7" t="s">
         <v>21</v>
@@ -4036,7 +4073,7 @@
         <v>2030</v>
       </c>
       <c r="AM45">
-        <v>15540.0813187964</v>
+        <v>14127.346653451301</v>
       </c>
       <c r="AP45" s="7" t="s">
         <v>21</v>
@@ -4049,7 +4086,7 @@
         <v>2040</v>
       </c>
       <c r="AS45">
-        <v>13804.9910177699</v>
+        <v>12549.991834336301</v>
       </c>
       <c r="AU45" s="7" t="s">
         <v>21</v>
@@ -4062,7 +4099,7 @@
         <v>2050</v>
       </c>
       <c r="AX45">
-        <v>12196.119700814201</v>
+        <v>11087.3815461947</v>
       </c>
       <c r="AZ45" t="str">
         <f t="shared" si="20"/>
@@ -4074,27 +4111,27 @@
       </c>
       <c r="BB45">
         <f t="shared" si="10"/>
-        <v>24888.396712212401</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="BC45">
         <f t="shared" si="11"/>
-        <v>17621.853096070899</v>
+        <v>16019.866450973501</v>
       </c>
       <c r="BD45">
         <f t="shared" si="12"/>
-        <v>16872.246964273298</v>
+        <v>15338.406331157514</v>
       </c>
       <c r="BE45">
         <f t="shared" si="13"/>
-        <v>16317.08538473622</v>
+        <v>14833.713986123867</v>
       </c>
       <c r="BF45">
         <f t="shared" si="14"/>
-        <v>14840.365344102642</v>
+        <v>13491.241221911523</v>
       </c>
       <c r="BG45">
         <f t="shared" si="15"/>
-        <v>13415.731670895622</v>
+        <v>12196.11970081417</v>
       </c>
       <c r="BJ45">
         <v>1</v>
@@ -4114,7 +4151,7 @@
         <v>2017</v>
       </c>
       <c r="X46">
-        <v>24888.396712212401</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="Z46" s="7" t="s">
         <v>21</v>
@@ -4127,7 +4164,7 @@
         <v>2020</v>
       </c>
       <c r="AC46">
-        <v>17621.853096070899</v>
+        <v>16019.866450973501</v>
       </c>
       <c r="AE46" s="7" t="s">
         <v>21</v>
@@ -4140,7 +4177,7 @@
         <v>2025</v>
       </c>
       <c r="AH46">
-        <v>16541.418592424801</v>
+        <v>15037.6532658407</v>
       </c>
       <c r="AJ46" s="7" t="s">
         <v>21</v>
@@ -4153,7 +4190,7 @@
         <v>2030</v>
       </c>
       <c r="AM46">
-        <v>15540.0813187964</v>
+        <v>14127.346653451301</v>
       </c>
       <c r="AP46" s="7" t="s">
         <v>21</v>
@@ -4166,7 +4203,7 @@
         <v>2040</v>
       </c>
       <c r="AS46">
-        <v>13804.9910177699</v>
+        <v>12549.991834336301</v>
       </c>
       <c r="AU46" s="7" t="s">
         <v>21</v>
@@ -4179,7 +4216,7 @@
         <v>2050</v>
       </c>
       <c r="AX46">
-        <v>12196.119700814201</v>
+        <v>11087.3815461947</v>
       </c>
       <c r="AZ46" t="str">
         <f t="shared" si="20"/>
@@ -4191,27 +4228,27 @@
       </c>
       <c r="BB46">
         <f t="shared" si="10"/>
-        <v>24888.396712212401</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="BC46">
         <f t="shared" si="11"/>
-        <v>17621.853096070899</v>
+        <v>16019.866450973501</v>
       </c>
       <c r="BD46">
         <f t="shared" si="12"/>
-        <v>16872.246964273298</v>
+        <v>15338.406331157514</v>
       </c>
       <c r="BE46">
         <f t="shared" si="13"/>
-        <v>16317.08538473622</v>
+        <v>14833.713986123867</v>
       </c>
       <c r="BF46">
         <f t="shared" si="14"/>
-        <v>14840.365344102642</v>
+        <v>13491.241221911523</v>
       </c>
       <c r="BG46">
         <f t="shared" si="15"/>
-        <v>13415.731670895622</v>
+        <v>12196.11970081417</v>
       </c>
       <c r="BJ46">
         <v>1</v>
@@ -4219,7 +4256,7 @@
     </row>
     <row r="47" spans="2:62" x14ac:dyDescent="0.25">
       <c r="C47" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="T47" t="s">
         <v>67</v>
@@ -4234,7 +4271,7 @@
         <v>2017</v>
       </c>
       <c r="X47">
-        <v>24888.396712212401</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="Z47" s="7" t="s">
         <v>21</v>
@@ -4247,7 +4284,7 @@
         <v>2020</v>
       </c>
       <c r="AC47">
-        <v>17621.853096070899</v>
+        <v>16019.866450973501</v>
       </c>
       <c r="AE47" s="7" t="s">
         <v>21</v>
@@ -4260,7 +4297,7 @@
         <v>2025</v>
       </c>
       <c r="AH47">
-        <v>16541.418592424801</v>
+        <v>15037.6532658407</v>
       </c>
       <c r="AJ47" s="7" t="s">
         <v>21</v>
@@ -4273,7 +4310,7 @@
         <v>2030</v>
       </c>
       <c r="AM47">
-        <v>15540.0813187964</v>
+        <v>14127.346653451301</v>
       </c>
       <c r="AP47" s="7" t="s">
         <v>21</v>
@@ -4286,7 +4323,7 @@
         <v>2040</v>
       </c>
       <c r="AS47">
-        <v>13804.9910177699</v>
+        <v>12549.991834336301</v>
       </c>
       <c r="AU47" s="7" t="s">
         <v>21</v>
@@ -4299,7 +4336,7 @@
         <v>2050</v>
       </c>
       <c r="AX47">
-        <v>12196.119700814201</v>
+        <v>11087.3815461947</v>
       </c>
       <c r="AZ47" t="str">
         <f t="shared" si="20"/>
@@ -4311,27 +4348,27 @@
       </c>
       <c r="BB47">
         <f t="shared" si="10"/>
-        <v>24888.396712212401</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="BC47">
         <f t="shared" si="11"/>
-        <v>17621.853096070899</v>
+        <v>16019.866450973501</v>
       </c>
       <c r="BD47">
         <f t="shared" si="12"/>
-        <v>16872.246964273298</v>
+        <v>15338.406331157514</v>
       </c>
       <c r="BE47">
         <f t="shared" si="13"/>
-        <v>16317.08538473622</v>
+        <v>14833.713986123867</v>
       </c>
       <c r="BF47">
         <f t="shared" si="14"/>
-        <v>14840.365344102642</v>
+        <v>13491.241221911523</v>
       </c>
       <c r="BG47">
         <f t="shared" si="15"/>
-        <v>13415.731670895622</v>
+        <v>12196.11970081417</v>
       </c>
       <c r="BJ47">
         <v>1</v>
@@ -4342,7 +4379,7 @@
         <v>11</v>
       </c>
       <c r="F48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G48" s="5">
         <f>1-L32</f>
@@ -4377,7 +4414,7 @@
         <v>2017</v>
       </c>
       <c r="X48">
-        <v>37547.150212389402</v>
+        <v>34133.772920354</v>
       </c>
       <c r="Z48" s="7" t="s">
         <v>21</v>
@@ -4390,7 +4427,7 @@
         <v>2020</v>
       </c>
       <c r="AC48">
-        <v>26584.692170796399</v>
+        <v>24167.901973451299</v>
       </c>
       <c r="AE48" s="7" t="s">
         <v>21</v>
@@ -4403,7 +4440,7 @@
         <v>2025</v>
       </c>
       <c r="AH48">
-        <v>24954.7263247788</v>
+        <v>22686.114840708</v>
       </c>
       <c r="AJ48" s="7" t="s">
         <v>21</v>
@@ -4416,7 +4453,7 @@
         <v>2030</v>
       </c>
       <c r="AM48">
-        <v>23444.088196460099</v>
+        <v>21312.8074513274</v>
       </c>
       <c r="AP48" s="7" t="s">
         <v>21</v>
@@ -4429,7 +4466,7 @@
         <v>2040</v>
       </c>
       <c r="AS48">
-        <v>20826.4950699115</v>
+        <v>18933.177336283199</v>
       </c>
       <c r="AU48" s="7" t="s">
         <v>21</v>
@@ -4442,7 +4479,7 @@
         <v>2050</v>
       </c>
       <c r="AX48">
-        <v>18399.318514159299</v>
+        <v>16726.653194690301</v>
       </c>
       <c r="AZ48" t="str">
         <f t="shared" si="20"/>
@@ -4454,27 +4491,27 @@
       </c>
       <c r="BB48">
         <f t="shared" si="10"/>
-        <v>37547.150212389402</v>
+        <v>34133.772920354</v>
       </c>
       <c r="BC48">
         <f t="shared" si="11"/>
-        <v>26584.692170796399</v>
+        <v>24167.901973451299</v>
       </c>
       <c r="BD48">
         <f t="shared" si="12"/>
-        <v>25453.820851274377</v>
+        <v>23139.837137522161</v>
       </c>
       <c r="BE48">
         <f t="shared" si="13"/>
-        <v>24616.292606283107</v>
+        <v>22378.44782389377</v>
       </c>
       <c r="BF48">
         <f t="shared" si="14"/>
-        <v>22388.48220015486</v>
+        <v>20353.165636504436</v>
       </c>
       <c r="BG48">
         <f t="shared" si="15"/>
-        <v>20239.25036557523</v>
+        <v>18399.318514159335</v>
       </c>
       <c r="BJ48">
         <v>1</v>
@@ -4486,7 +4523,7 @@
         <v>cemch_e</v>
       </c>
       <c r="F49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G49" s="5">
         <f>G48</f>
@@ -4521,7 +4558,7 @@
         <v>2017</v>
       </c>
       <c r="X49">
-        <v>24888.396712212401</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="Z49" s="7" t="s">
         <v>21</v>
@@ -4534,7 +4571,7 @@
         <v>2020</v>
       </c>
       <c r="AC49">
-        <v>17621.853096070899</v>
+        <v>16019.866450973501</v>
       </c>
       <c r="AE49" s="7" t="s">
         <v>21</v>
@@ -4547,7 +4584,7 @@
         <v>2025</v>
       </c>
       <c r="AH49">
-        <v>16541.418592424801</v>
+        <v>15037.6532658407</v>
       </c>
       <c r="AJ49" s="7" t="s">
         <v>21</v>
@@ -4560,7 +4597,7 @@
         <v>2030</v>
       </c>
       <c r="AM49">
-        <v>15540.0813187964</v>
+        <v>14127.346653451301</v>
       </c>
       <c r="AP49" s="7" t="s">
         <v>21</v>
@@ -4573,7 +4610,7 @@
         <v>2040</v>
       </c>
       <c r="AS49">
-        <v>13804.9910177699</v>
+        <v>12549.991834336301</v>
       </c>
       <c r="AU49" s="7" t="s">
         <v>21</v>
@@ -4586,7 +4623,7 @@
         <v>2050</v>
       </c>
       <c r="AX49">
-        <v>12196.119700814201</v>
+        <v>11087.3815461947</v>
       </c>
       <c r="AZ49" t="str">
         <f t="shared" si="20"/>
@@ -4598,27 +4635,27 @@
       </c>
       <c r="BB49">
         <f t="shared" si="10"/>
-        <v>24888.396712212401</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="BC49">
         <f t="shared" si="11"/>
-        <v>17621.853096070899</v>
+        <v>16019.866450973501</v>
       </c>
       <c r="BD49">
         <f t="shared" si="12"/>
-        <v>16872.246964273298</v>
+        <v>15338.406331157514</v>
       </c>
       <c r="BE49">
         <f t="shared" si="13"/>
-        <v>16317.08538473622</v>
+        <v>14833.713986123867</v>
       </c>
       <c r="BF49">
         <f t="shared" si="14"/>
-        <v>14840.365344102642</v>
+        <v>13491.241221911523</v>
       </c>
       <c r="BG49">
         <f t="shared" si="15"/>
-        <v>13415.731670895622</v>
+        <v>12196.11970081417</v>
       </c>
       <c r="BJ49">
         <v>1</v>
@@ -4630,7 +4667,7 @@
         <v>cemch_e</v>
       </c>
       <c r="F50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G50" s="5">
         <f>G49</f>
@@ -4665,7 +4702,7 @@
         <v>2017</v>
       </c>
       <c r="X50">
-        <v>6962.23719948902</v>
+        <v>6329.3065449900196</v>
       </c>
       <c r="Z50" s="7"/>
       <c r="AA50" s="9"/>
@@ -4689,7 +4726,7 @@
       </c>
       <c r="BB50">
         <f t="shared" si="10"/>
-        <v>6962.23719948902</v>
+        <v>6329.3065449900196</v>
       </c>
       <c r="BJ50">
         <v>1</v>
@@ -4701,7 +4738,7 @@
         <v>cemch_e</v>
       </c>
       <c r="F51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G51" s="5">
         <f>G50</f>
@@ -4728,7 +4765,7 @@
         <v>0.47538200339558578</v>
       </c>
       <c r="N51" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T51" s="9" t="s">
         <v>75</v>
@@ -4743,7 +4780,7 @@
         <v>2017</v>
       </c>
       <c r="X51">
-        <v>3093.2</v>
+        <v>2812</v>
       </c>
       <c r="Z51" s="7"/>
       <c r="AA51" s="9"/>
@@ -4761,7 +4798,7 @@
       </c>
       <c r="BB51">
         <f t="shared" si="10"/>
-        <v>3093.2</v>
+        <v>2812</v>
       </c>
       <c r="BJ51">
         <v>1</v>
@@ -4781,7 +4818,7 @@
         <v>2017</v>
       </c>
       <c r="X52">
-        <v>40688.264738559599</v>
+        <v>36989.331580508697</v>
       </c>
       <c r="Z52" s="7"/>
       <c r="AA52" s="9"/>
@@ -4799,7 +4836,7 @@
       </c>
       <c r="BB52">
         <f t="shared" si="10"/>
-        <v>40688.264738559599</v>
+        <v>36989.331580508697</v>
       </c>
       <c r="BJ52">
         <v>1</v>
@@ -4807,7 +4844,7 @@
     </row>
     <row r="53" spans="3:62" x14ac:dyDescent="0.25">
       <c r="C53" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T53" s="9" t="s">
         <v>79</v>
@@ -4822,7 +4859,7 @@
         <v>2017</v>
       </c>
       <c r="X53">
-        <v>20344.132435184001</v>
+        <v>18494.665850167301</v>
       </c>
       <c r="Z53" s="7"/>
       <c r="AA53" s="9"/>
@@ -4840,7 +4877,7 @@
       </c>
       <c r="BB53">
         <f t="shared" si="10"/>
-        <v>20344.132435184001</v>
+        <v>18494.665850167301</v>
       </c>
       <c r="BJ53">
         <v>1</v>
@@ -4848,10 +4885,10 @@
     </row>
     <row r="54" spans="3:62" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G54" s="6">
         <f>1-O32</f>
@@ -4894,7 +4931,7 @@
         <v>2017</v>
       </c>
       <c r="X54">
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="Z54" s="7"/>
       <c r="AA54" s="9"/>
@@ -4912,7 +4949,7 @@
       </c>
       <c r="BB54">
         <f t="shared" si="10"/>
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="BJ54">
         <v>1</v>
@@ -4920,10 +4957,10 @@
     </row>
     <row r="55" spans="3:62" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G55" s="6">
         <f>G54</f>
@@ -4962,7 +4999,7 @@
         <v>2017</v>
       </c>
       <c r="X55">
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="Z55" s="7"/>
       <c r="AA55" s="9"/>
@@ -4980,7 +5017,7 @@
       </c>
       <c r="BB55">
         <f t="shared" si="10"/>
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="BJ55">
         <v>1</v>
@@ -4988,10 +5025,10 @@
     </row>
     <row r="56" spans="3:62" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F56" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G56" s="6">
         <f>G55</f>
@@ -5029,7 +5066,7 @@
         <v>2017</v>
       </c>
       <c r="X56">
-        <v>15536.865868655899</v>
+        <v>14124.4235169599</v>
       </c>
       <c r="Z56" s="7"/>
       <c r="AA56" s="9"/>
@@ -5047,7 +5084,7 @@
       </c>
       <c r="BB56">
         <f t="shared" si="10"/>
-        <v>15536.865868655899</v>
+        <v>14124.4235169599</v>
       </c>
       <c r="BJ56">
         <v>1</v>
@@ -5055,10 +5092,10 @@
     </row>
     <row r="57" spans="3:62" x14ac:dyDescent="0.25">
       <c r="C57" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F57" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G57" s="6">
         <f>G56</f>
@@ -5085,7 +5122,7 @@
         <v>0.93842364532019706</v>
       </c>
       <c r="N57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T57" s="9" t="s">
         <v>87</v>
@@ -5100,7 +5137,7 @@
         <v>2017</v>
       </c>
       <c r="X57">
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="AZ57" t="str">
         <f t="shared" si="20"/>
@@ -5112,7 +5149,7 @@
       </c>
       <c r="BB57">
         <f t="shared" si="10"/>
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="BJ57">
         <v>1</v>
@@ -5132,7 +5169,7 @@
         <v>2017</v>
       </c>
       <c r="X58">
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="AZ58" t="str">
         <f t="shared" si="20"/>
@@ -5144,7 +5181,7 @@
       </c>
       <c r="BB58">
         <f t="shared" si="10"/>
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="BJ58">
         <v>1</v>
@@ -5152,7 +5189,7 @@
     </row>
     <row r="59" spans="3:62" x14ac:dyDescent="0.25">
       <c r="C59" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="T59" s="9" t="s">
         <v>91</v>
@@ -5167,7 +5204,7 @@
         <v>2017</v>
       </c>
       <c r="X59">
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="AZ59" t="str">
         <f t="shared" si="20"/>
@@ -5179,7 +5216,7 @@
       </c>
       <c r="BB59">
         <f t="shared" si="10"/>
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="BJ59">
         <v>1</v>
@@ -5187,10 +5224,10 @@
     </row>
     <row r="60" spans="3:62" x14ac:dyDescent="0.25">
       <c r="C60" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F60" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G60" s="6">
         <f>1-N32</f>
@@ -5233,7 +5270,7 @@
         <v>2017</v>
       </c>
       <c r="X60">
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="AZ60" t="str">
         <f t="shared" si="20"/>
@@ -5245,7 +5282,7 @@
       </c>
       <c r="BB60">
         <f t="shared" si="10"/>
-        <v>9670.4719226068701</v>
+        <v>8791.3381114607892</v>
       </c>
       <c r="BJ60">
         <v>1</v>
@@ -5257,7 +5294,7 @@
         <v>cmetp</v>
       </c>
       <c r="F61" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G61" s="6">
         <f>G60</f>
@@ -5296,7 +5333,7 @@
         <v>2017</v>
       </c>
       <c r="X61">
-        <v>15536.865868655899</v>
+        <v>14124.4235169599</v>
       </c>
       <c r="AZ61" t="str">
         <f t="shared" si="20"/>
@@ -5308,7 +5345,7 @@
       </c>
       <c r="BB61">
         <f t="shared" si="10"/>
-        <v>15536.865868655899</v>
+        <v>14124.4235169599</v>
       </c>
       <c r="BJ61">
         <v>1</v>
@@ -5320,7 +5357,7 @@
         <v>cmetp</v>
       </c>
       <c r="F62" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G62" s="6">
         <f>G61</f>
@@ -5359,7 +5396,7 @@
         <v>2017</v>
       </c>
       <c r="X62">
-        <v>15536.865868655899</v>
+        <v>14124.4235169599</v>
       </c>
       <c r="AZ62" t="str">
         <f t="shared" si="20"/>
@@ -5371,7 +5408,7 @@
       </c>
       <c r="BB62">
         <f t="shared" si="10"/>
-        <v>15536.865868655899</v>
+        <v>14124.4235169599</v>
       </c>
       <c r="BJ62">
         <v>1</v>
@@ -5383,7 +5420,7 @@
         <v>cmetp</v>
       </c>
       <c r="F63" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G63" s="6">
         <f>G62</f>
@@ -5410,7 +5447,7 @@
         <v>0.76065573770491801</v>
       </c>
       <c r="N63" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="T63" s="9" t="s">
         <v>99</v>
@@ -5425,7 +5462,7 @@
         <v>2017</v>
       </c>
       <c r="X63">
-        <v>40688.264738559599</v>
+        <v>36989.331580508697</v>
       </c>
       <c r="AZ63" t="str">
         <f t="shared" si="20"/>
@@ -5437,7 +5474,7 @@
       </c>
       <c r="BB63">
         <f t="shared" si="10"/>
-        <v>40688.264738559599</v>
+        <v>36989.331580508697</v>
       </c>
       <c r="BJ63">
         <v>1</v>
@@ -5457,7 +5494,7 @@
         <v>2017</v>
       </c>
       <c r="X64">
-        <v>20344.132435184001</v>
+        <v>18494.665850167301</v>
       </c>
       <c r="AZ64" t="str">
         <f t="shared" si="20"/>
@@ -5469,7 +5506,7 @@
       </c>
       <c r="BB64">
         <f t="shared" si="10"/>
-        <v>20344.132435184001</v>
+        <v>18494.665850167301</v>
       </c>
       <c r="BJ64">
         <v>1</v>
@@ -5477,7 +5514,7 @@
     </row>
     <row r="65" spans="3:62" x14ac:dyDescent="0.25">
       <c r="C65" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T65" s="9" t="s">
         <v>103</v>
@@ -5492,7 +5529,7 @@
         <v>2017</v>
       </c>
       <c r="X65">
-        <v>10172.066217592001</v>
+        <v>9247.3329250836705</v>
       </c>
       <c r="AZ65" t="str">
         <f t="shared" si="20"/>
@@ -5504,7 +5541,7 @@
       </c>
       <c r="BB65">
         <f t="shared" si="10"/>
-        <v>10172.066217592001</v>
+        <v>9247.3329250836705</v>
       </c>
       <c r="BJ65">
         <v>1</v>
@@ -5512,7 +5549,7 @@
     </row>
     <row r="66" spans="3:62" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G66" s="6">
         <v>0</v>
@@ -5537,7 +5574,7 @@
     </row>
     <row r="67" spans="3:62" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G67" s="6">
         <v>0</v>
@@ -5560,7 +5597,7 @@
     </row>
     <row r="68" spans="3:62" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G68" s="6">
         <v>0</v>
@@ -5583,7 +5620,7 @@
     </row>
     <row r="69" spans="3:62" x14ac:dyDescent="0.25">
       <c r="F69" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G69" s="6">
         <v>0</v>
@@ -5606,24 +5643,24 @@
     </row>
     <row r="79" spans="3:62" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
+        <v>129</v>
+      </c>
+      <c r="H79" t="s">
         <v>130</v>
-      </c>
-      <c r="H79" t="s">
-        <v>131</v>
       </c>
       <c r="I79" t="s">
         <v>9</v>
       </c>
       <c r="J79" t="s">
+        <v>131</v>
+      </c>
+      <c r="K79" t="s">
         <v>132</v>
-      </c>
-      <c r="K79" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="80" spans="3:62" x14ac:dyDescent="0.25">
       <c r="F80" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G80">
         <v>100</v>
@@ -5651,7 +5688,7 @@
     </row>
     <row r="82" spans="6:10" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G82">
         <v>36.5</v>
@@ -5685,5 +5722,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added another localisation scenario
For high local content, medium price increases. for sensitivity.
Revamped scenario selector for the others too.
</commit_message>
<xml_diff>
--- a/suppxls/Scen_Localisation-Hi.xlsx
+++ b/suppxls/Scen_Localisation-Hi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E8D8D32-14B9-4278-8754-C8DE62A6F923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9E70F3-685F-4D83-90E2-0F4309B7FBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{232E471A-D1BC-46EA-822F-4A9C8F9BFC34}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{232E471A-D1BC-46EA-822F-4A9C8F9BFC34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="139">
   <si>
     <t>~TFM_INS-TS</t>
   </si>
@@ -462,6 +462,15 @@
   </si>
   <si>
     <t>TFM_FILL</t>
+  </si>
+  <si>
+    <t>Localisation</t>
+  </si>
+  <si>
+    <t>Cost increase</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -471,7 +480,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,6 +556,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -561,7 +578,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -664,6 +681,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -673,7 +705,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
@@ -710,6 +742,9 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="5"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="5" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Heading 4" xfId="2" builtinId="19"/>
@@ -737,15 +772,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>48</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>210608</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>50</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>423333</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -760,8 +795,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="29860875" y="1743075"/>
-          <a:ext cx="1323975" cy="219075"/>
+          <a:off x="30828191" y="3757083"/>
+          <a:ext cx="1440392" cy="522817"/>
         </a:xfrm>
         <a:prstGeom prst="rightArrow">
           <a:avLst/>
@@ -1108,14 +1143,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C1C3BE-43A3-4F6E-B7BA-55F1C4F1EF02}">
-  <dimension ref="B2:BL83"/>
+  <dimension ref="B1:BL83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
@@ -1123,22 +1159,38 @@
     <col min="53" max="53" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C2" s="10" t="s">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="32" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="3" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C3" s="30" t="s">
+      <c r="C1" s="18"/>
+    </row>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="19"/>
+      <c r="C2" s="22"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="33" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4" s="33" t="s">
+        <v>112</v>
+      </c>
       <c r="E4" s="10" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="19"/>
+      <c r="C5" s="22"/>
       <c r="G5" s="12">
         <v>2017</v>
       </c>
@@ -1158,7 +1210,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
       <c r="E6" t="s">
         <v>8</v>
       </c>
@@ -1190,7 +1244,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="7" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>11</v>
       </c>
@@ -1222,7 +1276,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="8" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>123</v>
       </c>
@@ -1254,7 +1308,7 @@
         <v>0.78098360655737697</v>
       </c>
     </row>
-    <row r="9" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>120</v>
       </c>
@@ -1286,12 +1340,12 @@
         <v>0.94827586206896552</v>
       </c>
     </row>
-    <row r="12" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C12" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1301,7 +1355,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>1</v>
       </c>
@@ -1333,7 +1387,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="16" spans="3:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>3</v>
       </c>
@@ -1396,7 +1450,7 @@
         <v>0.52461799660441422</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" ref="I17:L17" si="5">1-I7</f>
+        <f t="shared" ref="I17:K17" si="5">1-I7</f>
         <v>0.44999999999999996</v>
       </c>
       <c r="J17" s="5">
@@ -1408,7 +1462,7 @@
         <v>0.25</v>
       </c>
       <c r="L17" s="5">
-        <f t="shared" si="5"/>
+        <f>1-L7</f>
         <v>0.15000000000000002</v>
       </c>
     </row>
@@ -1551,11 +1605,11 @@
         <v>108</v>
       </c>
       <c r="BB22" s="4">
-        <f>SUMIF($F$66:$F$69,$C$3,G66:G69)</f>
+        <f>SUMIF($F$66:$F$69,$C$4,G66:G69)</f>
         <v>0</v>
       </c>
       <c r="BC22" s="4">
-        <f t="shared" ref="BC22:BG22" si="8">SUMIF($F$66:$F$69,$C$3,H66:H69)</f>
+        <f t="shared" ref="BC22:BG22" si="8">SUMIF($F$66:$F$69,$C$4,H66:H69)</f>
         <v>0</v>
       </c>
       <c r="BD22" s="4">
@@ -3153,8 +3207,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:62" x14ac:dyDescent="0.25">
-      <c r="B38" s="10" t="s">
+    <row r="38" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B38" s="31" t="s">
         <v>114</v>
       </c>
       <c r="T38" s="9" t="s">
@@ -5512,8 +5566,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="3:62" x14ac:dyDescent="0.25">
-      <c r="C65" s="10" t="s">
+    <row r="65" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B65" s="31" t="s">
         <v>134</v>
       </c>
       <c r="T65" s="9" t="s">
@@ -5547,7 +5601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:62" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
         <v>111</v>
       </c>
@@ -5564,15 +5618,15 @@
         <v>0.05</v>
       </c>
       <c r="K66" s="6">
-        <v>7.4999999999999997E-2</v>
+        <v>0.125</v>
       </c>
       <c r="L66" s="6">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="V66" s="9"/>
       <c r="W66" s="9"/>
     </row>
-    <row r="67" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:62" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
         <v>112</v>
       </c>
@@ -5583,19 +5637,19 @@
         <v>0</v>
       </c>
       <c r="I67" s="6">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="J67" s="6">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="K67" s="6">
-        <v>0.05</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="L67" s="6">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="68" spans="3:62" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:62" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
         <v>113</v>
       </c>
@@ -5605,22 +5659,22 @@
       <c r="H68" s="6">
         <v>0</v>
       </c>
-      <c r="I68" s="28">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="J68" s="6">
+      <c r="I68" s="6">
         <v>0.01</v>
       </c>
-      <c r="K68" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="L68" s="6">
+      <c r="J68" s="5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K68" s="5">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L68" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="69" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:62" x14ac:dyDescent="0.25">
       <c r="F69" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="G69" s="6">
         <v>0</v>
@@ -5641,7 +5695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:62" x14ac:dyDescent="0.25">
       <c r="G79" t="s">
         <v>129</v>
       </c>
@@ -5658,7 +5712,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="80" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:62" x14ac:dyDescent="0.25">
       <c r="F80" t="s">
         <v>128</v>
       </c>
@@ -5715,9 +5769,12 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{28F83205-2B6D-4B86-9C9B-CC3DB94DE282}">
       <formula1>$F$41:$F$44</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{B1584D95-3338-4846-9756-AAD3A2F15D0C}">
+      <formula1>$F$66:$F$69</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Elc Costs updated. Still need to push diesel use up for hist years
</commit_message>
<xml_diff>
--- a/suppxls/Scen_Localisation-Hi.xlsx
+++ b/suppxls/Scen_Localisation-Hi.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <workbookPr updateLinks="never" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE_Veda\suppxls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9E70F3-685F-4D83-90E2-0F4309B7FBC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{232E471A-D1BC-46EA-822F-4A9C8F9BFC34}"/>
+    <workbookView xWindow="-825" yWindow="-18675" windowWidth="28770" windowHeight="15600" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,10 +43,12 @@
   <commentList>
     <comment ref="U24" authorId="0" shapeId="0" xr:uid="{BFF637BF-F295-4BD2-8A3C-4C0D24997E80}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This must be re-activated when Reference costs are changed. One must leave it de-activated for High Localisation scenarios</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -461,9 +463,6 @@
     <t>Cost Increase</t>
   </si>
   <si>
-    <t>TFM_FILL</t>
-  </si>
-  <si>
     <t>Localisation</t>
   </si>
   <si>
@@ -471,6 +470,9 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>~TFM_FILL</t>
   </si>
 </sst>
 </file>
@@ -480,7 +482,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,11 +491,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -575,6 +576,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -584,86 +586,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -679,14 +601,85 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
@@ -694,68 +687,171 @@
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="24">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="22" applyFont="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="22" applyFont="1">
+      <alignment/>
+      <protection/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="15" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="15" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="15" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="9" xfId="5"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="23"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="23" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Heading 4" xfId="2" builtinId="19"/>
-    <cellStyle name="Input" xfId="5" builtinId="20"/>
+  <cellStyles count="10">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 13" xfId="4" xr:uid="{8D155F1E-CE31-43C4-B63E-69EA0E23AFF4}"/>
-    <cellStyle name="Normal 2" xfId="3" xr:uid="{114B2D43-D8F0-4A77-911E-913BD0BF594C}"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Normal 2" xfId="21"/>
+    <cellStyle name="Normal 13" xfId="22"/>
+    <cellStyle name="Input" xfId="23" builtinId="20"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -768,7 +864,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>48</xdr:col>
@@ -782,12 +878,12 @@
       <xdr:row>22</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Arrow: Right 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A247403-132B-398E-E96F-241036AD5818}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6a247403-132b-398e-e96f-241036ad5818}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -795,12 +891,10 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="30828191" y="3757083"/>
-          <a:ext cx="1440392" cy="522817"/>
+          <a:off x="31089600" y="3752850"/>
+          <a:ext cx="1428750" cy="523875"/>
         </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rightArrow"/>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -815,7 +909,7 @@
           <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="bg1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -839,9 +933,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -879,7 +973,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -985,7 +1079,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1127,13 +1221,13 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/threadedComments/threadedComments1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="U24" dT="2023-12-19T09:22:03.61" personId="{B5E69722-C63D-4CBF-877A-AF5854BD44E9}" id="{BFF637BF-F295-4BD2-8A3C-4C0D24997E80}">
     <text>This must be re-activated when Reference costs are changed. One must leave it de-activated for High Localisation scenarios</text>
@@ -1142,44 +1236,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C1C3BE-43A3-4F6E-B7BA-55F1C4F1EF02}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10C1C3BE-43A3-4F6E-B7BA-55F1C4F1EF02}">
   <dimension ref="B1:BL83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" customWidth="1"/>
-    <col min="53" max="53" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="13.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="11.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="9.85714285714286" customWidth="1"/>
+    <col min="6" max="6" width="19.4285714285714" customWidth="1"/>
+    <col min="53" max="53" width="16.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:3" ht="15">
       <c r="B1" s="32" t="s">
         <v>119</v>
       </c>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="15">
       <c r="B2" s="19"/>
       <c r="C2" s="22"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="15">
       <c r="B3" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C3" s="33" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" ht="15">
       <c r="B4" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>112</v>
@@ -1188,7 +1282,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="15">
       <c r="B5" s="19"/>
       <c r="C5" s="22"/>
       <c r="G5" s="12">
@@ -1210,7 +1304,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" ht="15">
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
       <c r="E6" t="s">
@@ -1232,8 +1326,8 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J6" s="27">
-        <f t="shared" ref="J6:L6" si="0">SUMIFS(J$41:J$63,$C$41:$C$63,$E16,$F$41:$F$63,$C$3)</f>
-        <v>0.7</v>
+        <f t="shared" si="0" ref="J6:L6">SUMIFS(J$41:J$63,$C$41:$C$63,$E16,$F$41:$F$63,$C$3)</f>
+        <v>0.69999999999999996</v>
       </c>
       <c r="K6" s="27">
         <f t="shared" si="0"/>
@@ -1241,10 +1335,10 @@
       </c>
       <c r="L6" s="27">
         <f t="shared" si="0"/>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.84999999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="5:12" ht="15">
       <c r="E7" t="s">
         <v>11</v>
       </c>
@@ -1260,12 +1354,12 @@
         <v>0.47538200339558578</v>
       </c>
       <c r="I7" s="27">
-        <f t="shared" ref="I7:L7" si="1">SUMIFS(I$41:I$63,$C$41:$C$63,$E17,$F$41:$F$63,$C$3)</f>
+        <f t="shared" si="1" ref="I7:L7">SUMIFS(I$41:I$63,$C$41:$C$63,$E17,$F$41:$F$63,$C$3)</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="J7" s="27">
         <f t="shared" si="1"/>
-        <v>0.7</v>
+        <v>0.69999999999999996</v>
       </c>
       <c r="K7" s="27">
         <f t="shared" si="1"/>
@@ -1273,10 +1367,10 @@
       </c>
       <c r="L7" s="27">
         <f t="shared" si="1"/>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.84999999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="5:12" ht="15">
       <c r="E8" t="s">
         <v>123</v>
       </c>
@@ -1292,7 +1386,7 @@
         <v>0.76065573770491801</v>
       </c>
       <c r="I8" s="27">
-        <f t="shared" ref="I8:L8" si="2">SUMIFS(I$41:I$63,$C$41:$C$63,$E18,$F$41:$F$63,$C$3)</f>
+        <f t="shared" si="2" ref="I8:L8">SUMIFS(I$41:I$63,$C$41:$C$63,$E18,$F$41:$F$63,$C$3)</f>
         <v>0.76065573770491801</v>
       </c>
       <c r="J8" s="27">
@@ -1308,7 +1402,7 @@
         <v>0.78098360655737697</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:12" ht="15">
       <c r="E9" t="s">
         <v>120</v>
       </c>
@@ -1324,7 +1418,7 @@
         <v>0.93842364532019706</v>
       </c>
       <c r="I9" s="27">
-        <f t="shared" ref="I9:L9" si="3">SUMIFS(I$41:I$63,$C$41:$C$63,$E19,$F$41:$F$63,$C$3)</f>
+        <f t="shared" si="3" ref="I9:L9">SUMIFS(I$41:I$63,$C$41:$C$63,$E19,$F$41:$F$63,$C$3)</f>
         <v>0.93842364532019706</v>
       </c>
       <c r="J9" s="27">
@@ -1340,12 +1434,12 @@
         <v>0.94827586206896552</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:3" ht="15">
       <c r="C12" s="10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:8" ht="15">
       <c r="C14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1355,7 +1449,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:12" ht="15">
       <c r="C15" s="2" t="s">
         <v>1</v>
       </c>
@@ -1387,7 +1481,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:14" ht="15">
       <c r="C16" s="3" t="s">
         <v>3</v>
       </c>
@@ -1413,7 +1507,7 @@
         <v>0.44999999999999996</v>
       </c>
       <c r="J16" s="5">
-        <f t="shared" ref="J16:L16" si="4">1-J6</f>
+        <f t="shared" si="4" ref="J16:L16">1-J6</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="K16" s="5">
@@ -1428,7 +1522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:12" ht="15">
       <c r="C17" s="3" t="s">
         <v>4</v>
       </c>
@@ -1450,7 +1544,7 @@
         <v>0.52461799660441422</v>
       </c>
       <c r="I17" s="5">
-        <f t="shared" ref="I17:K17" si="5">1-I7</f>
+        <f t="shared" si="5" ref="I17:K17">1-I7</f>
         <v>0.44999999999999996</v>
       </c>
       <c r="J17" s="5">
@@ -1466,7 +1560,7 @@
         <v>0.15000000000000002</v>
       </c>
     </row>
-    <row r="18" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:64" ht="15">
       <c r="C18" t="s">
         <v>121</v>
       </c>
@@ -1488,7 +1582,7 @@
         <v>0.23934426229508196</v>
       </c>
       <c r="I18" s="5">
-        <f t="shared" ref="I18:L18" si="6">1-I8</f>
+        <f t="shared" si="6" ref="I18:L18">1-I8</f>
         <v>0.23934426229508199</v>
       </c>
       <c r="J18" s="5">
@@ -1551,7 +1645,7 @@
       <c r="BK18" s="13"/>
       <c r="BL18" s="13"/>
     </row>
-    <row r="19" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:20" ht="15">
       <c r="C19" t="s">
         <v>122</v>
       </c>
@@ -1566,38 +1660,38 @@
       </c>
       <c r="G19" s="6">
         <f>O32</f>
-        <v>6.1576354679802957E-2</v>
+        <v>0.061576354679802957</v>
       </c>
       <c r="H19" s="5">
         <f>G19</f>
-        <v>6.1576354679802957E-2</v>
+        <v>0.061576354679802957</v>
       </c>
       <c r="I19" s="5">
-        <f t="shared" ref="I19:L19" si="7">1-I9</f>
-        <v>6.1576354679802936E-2</v>
+        <f t="shared" si="7" ref="I19:L19">1-I9</f>
+        <v>0.061576354679802936</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" si="7"/>
-        <v>5.1724137931034475E-2</v>
+        <v>0.051724137931034475</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="7"/>
-        <v>5.1724137931034475E-2</v>
+        <v>0.051724137931034475</v>
       </c>
       <c r="L19" s="5">
         <f t="shared" si="7"/>
-        <v>5.1724137931034475E-2</v>
+        <v>0.051724137931034475</v>
       </c>
       <c r="T19" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="52:52" ht="15">
       <c r="AZ21" s="14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="20:59" ht="15">
       <c r="T22" s="14" t="s">
         <v>106</v>
       </c>
@@ -1609,7 +1703,7 @@
         <v>0</v>
       </c>
       <c r="BC22" s="4">
-        <f t="shared" ref="BC22:BG22" si="8">SUMIF($F$66:$F$69,$C$4,H66:H69)</f>
+        <f t="shared" si="8" ref="BC22:BG22">SUMIF($F$66:$F$69,$C$4,H66:H69)</f>
         <v>0</v>
       </c>
       <c r="BD22" s="4">
@@ -1618,43 +1712,43 @@
       </c>
       <c r="BE22" s="4">
         <f t="shared" si="8"/>
-        <v>0.05</v>
+        <v>0.050000000000000003</v>
       </c>
       <c r="BF22" s="4">
         <f t="shared" si="8"/>
-        <v>7.4999999999999997E-2</v>
+        <v>0.074999999999999997</v>
       </c>
       <c r="BG22" s="4">
         <f t="shared" si="8"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="23" spans="3:64" x14ac:dyDescent="0.25">
+        <v>0.10000000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="14:14" ht="15">
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="21:62" ht="15">
       <c r="U24" s="30" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="Z24" t="str">
         <f>U24</f>
-        <v>TFM_FILL</v>
+        <v>~TFM_FILL</v>
       </c>
       <c r="AE24" t="str">
         <f>Z24</f>
-        <v>TFM_FILL</v>
+        <v>~TFM_FILL</v>
       </c>
       <c r="AJ24" t="str">
         <f>AE24</f>
-        <v>TFM_FILL</v>
+        <v>~TFM_FILL</v>
       </c>
       <c r="AP24" t="str">
         <f>AJ24</f>
-        <v>TFM_FILL</v>
+        <v>~TFM_FILL</v>
       </c>
       <c r="AU24" t="str">
         <f>AP24</f>
-        <v>TFM_FILL</v>
+        <v>~TFM_FILL</v>
       </c>
       <c r="AZ24" s="1" t="s">
         <v>0</v>
@@ -1663,7 +1757,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="20:59" ht="15">
       <c r="T25" s="8" t="s">
         <v>22</v>
       </c>
@@ -1768,7 +1862,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="26" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="20:62" ht="15">
       <c r="T26" s="9" t="s">
         <v>25</v>
       </c>
@@ -1818,7 +1912,7 @@
         <v>21</v>
       </c>
       <c r="AQ26" s="9" t="str">
-        <f t="shared" ref="AQ26:AQ49" si="9">V26</f>
+        <f t="shared" si="9" ref="AQ26:AQ49">V26</f>
         <v>ETCLEMEDU-N</v>
       </c>
       <c r="AR26" s="7">
@@ -1843,34 +1937,34 @@
         <v>ETCLEMEDU-N</v>
       </c>
       <c r="BB26">
-        <f t="shared" ref="BB26:BB65" si="10">IF($BJ26,X26*(1+$BB$22),X26)</f>
+        <f t="shared" si="10" ref="BB26:BB65">IF($BJ26,X26*(1+$BB$22),X26)</f>
         <v>51359.8538564517</v>
       </c>
       <c r="BC26" t="str">
-        <f t="shared" ref="BC26:BC49" si="11">IF(IF($BJ26,AC26*(1+BC$22),AC26)=0,"",IF($BJ26,AC26*(1+BC$22),AC26))</f>
+        <f t="shared" si="11" ref="BC26:BC49">IF(IF($BJ26,AC26*(1+BC$22),AC26)=0,"",IF($BJ26,AC26*(1+BC$22),AC26))</f>
         <v/>
       </c>
       <c r="BD26" t="str">
-        <f t="shared" ref="BD26:BD49" si="12">IF(IF($BJ26,AH26*(1+BD$22),AH26)=0,"",IF($BJ26,AH26*(1+BD$22),AH26))</f>
+        <f t="shared" si="12" ref="BD26:BD49">IF(IF($BJ26,AH26*(1+BD$22),AH26)=0,"",IF($BJ26,AH26*(1+BD$22),AH26))</f>
         <v/>
       </c>
       <c r="BE26" t="str">
-        <f t="shared" ref="BE26:BE49" si="13">IF(IF($BJ26,AM26*(1+BE$22),AM26)=0,"",IF($BJ26,AM26*(1+BE$22),AM26))</f>
+        <f t="shared" si="13" ref="BE26:BE49">IF(IF($BJ26,AM26*(1+BE$22),AM26)=0,"",IF($BJ26,AM26*(1+BE$22),AM26))</f>
         <v/>
       </c>
       <c r="BF26" t="str">
-        <f t="shared" ref="BF26:BF49" si="14">IF(IF($BJ26,AS26*(1+BF$22),AS26)=0,"",IF($BJ26,AS26*(1+BF$22),AS26))</f>
+        <f t="shared" si="14" ref="BF26:BF49">IF(IF($BJ26,AS26*(1+BF$22),AS26)=0,"",IF($BJ26,AS26*(1+BF$22),AS26))</f>
         <v/>
       </c>
       <c r="BG26" t="str">
-        <f t="shared" ref="BG26:BG49" si="15">IF(IF($BJ26,AX26*(1+BG$22),AX26)=0,"",IF($BJ26,AX26*(1+BG$22),AX26))</f>
+        <f t="shared" si="15" ref="BG26:BG49">IF(IF($BJ26,AX26*(1+BG$22),AX26)=0,"",IF($BJ26,AX26*(1+BG$22),AX26))</f>
         <v/>
       </c>
       <c r="BJ26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="27" spans="20:62" ht="15">
       <c r="T27" s="9" t="s">
         <v>27</v>
       </c>
@@ -1890,7 +1984,7 @@
         <v>21</v>
       </c>
       <c r="AA27" s="9" t="str">
-        <f t="shared" ref="AA27:AA49" si="16">V27</f>
+        <f t="shared" si="16" ref="AA27:AA49">V27</f>
         <v>ETCLEKUSI-N</v>
       </c>
       <c r="AB27" s="7">
@@ -1900,7 +1994,7 @@
         <v>21</v>
       </c>
       <c r="AF27" s="9" t="str">
-        <f t="shared" ref="AF27:AF49" si="17">AA27</f>
+        <f t="shared" si="17" ref="AF27:AF49">AA27</f>
         <v>ETCLEKUSI-N</v>
       </c>
       <c r="AG27" s="7">
@@ -1910,7 +2004,7 @@
         <v>21</v>
       </c>
       <c r="AK27" s="9" t="str">
-        <f t="shared" ref="AK27:AK49" si="18">AF27</f>
+        <f t="shared" si="18" ref="AK27:AK49">AF27</f>
         <v>ETCLEKUSI-N</v>
       </c>
       <c r="AL27" s="7">
@@ -1930,18 +2024,18 @@
         <v>21</v>
       </c>
       <c r="AV27" s="9" t="str">
-        <f t="shared" ref="AV27:AV49" si="19">V27</f>
+        <f t="shared" si="19" ref="AV27:AV49">V27</f>
         <v>ETCLEKUSI-N</v>
       </c>
       <c r="AW27" s="7">
         <v>2050</v>
       </c>
       <c r="AZ27" t="str">
-        <f t="shared" ref="AZ27:AZ65" si="20">U27</f>
+        <f t="shared" si="20" ref="AZ27:AZ65">U27</f>
         <v>NCAP_COST</v>
       </c>
       <c r="BA27" t="str">
-        <f t="shared" ref="BA27:BA65" si="21">V27</f>
+        <f t="shared" si="21" ref="BA27:BA65">V27</f>
         <v>ETCLEKUSI-N</v>
       </c>
       <c r="BB27">
@@ -1972,7 +2066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:62" ht="15">
       <c r="C28" s="10" t="s">
         <v>17</v>
       </c>
@@ -2077,7 +2171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:62" ht="15">
       <c r="C29" s="16"/>
       <c r="D29" s="17" t="s">
         <v>12</v>
@@ -2200,7 +2294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:62" ht="15">
       <c r="C30" s="19"/>
       <c r="D30" t="s">
         <v>13</v>
@@ -2328,7 +2422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:62" ht="15">
       <c r="C31" s="19" t="s">
         <v>15</v>
       </c>
@@ -2467,7 +2561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="3:64" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:62" ht="15">
       <c r="C32" s="19">
         <v>2019</v>
       </c>
@@ -2478,14 +2572,14 @@
         <v>3.33</v>
       </c>
       <c r="F32">
-        <v>5.6</v>
+        <v>5.60</v>
       </c>
       <c r="G32">
         <v>2.96</v>
       </c>
       <c r="I32">
         <f>D32+F32</f>
-        <v>11.78</v>
+        <v>11.779999999999999</v>
       </c>
       <c r="J32">
         <f>E32+G32</f>
@@ -2505,7 +2599,7 @@
       </c>
       <c r="O32" s="24">
         <f>G81</f>
-        <v>6.1576354679802957E-2</v>
+        <v>0.061576354679802957</v>
       </c>
       <c r="T32" s="9" t="s">
         <v>37</v>
@@ -2608,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:62" ht="15">
       <c r="C33" s="19">
         <v>2020</v>
       </c>
@@ -2619,10 +2713,10 @@
         <v>8.48</v>
       </c>
       <c r="F33">
-        <v>6.5</v>
+        <v>6.50</v>
       </c>
       <c r="G33">
-        <v>7.2</v>
+        <v>7.20</v>
       </c>
       <c r="O33" s="22"/>
       <c r="T33" s="9" t="s">
@@ -2638,7 +2732,7 @@
         <v>2017</v>
       </c>
       <c r="X33">
-        <v>81279.984337530506</v>
+        <v>81278.984337530506</v>
       </c>
       <c r="Z33" s="7" t="s">
         <v>21</v>
@@ -2651,7 +2745,7 @@
         <v>2020</v>
       </c>
       <c r="AC33">
-        <v>73998.533002521595</v>
+        <v>81279.984337530506</v>
       </c>
       <c r="AE33" s="7" t="s">
         <v>21</v>
@@ -2715,11 +2809,11 @@
       </c>
       <c r="BB33">
         <f t="shared" si="10"/>
-        <v>81279.984337530506</v>
+        <v>81278.984337530506</v>
       </c>
       <c r="BC33">
         <f t="shared" si="11"/>
-        <v>73998.533002521595</v>
+        <v>81279.984337530506</v>
       </c>
       <c r="BD33">
         <f t="shared" si="12"/>
@@ -2741,7 +2835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:62" ht="15">
       <c r="C34" s="25"/>
       <c r="D34" s="13"/>
       <c r="E34" s="13"/>
@@ -2768,7 +2862,7 @@
         <v>2017</v>
       </c>
       <c r="X34">
-        <v>19505.013097345101</v>
+        <v>48762.532743362797</v>
       </c>
       <c r="Z34" s="7" t="s">
         <v>21</v>
@@ -2781,7 +2875,7 @@
         <v>2020</v>
       </c>
       <c r="AC34">
-        <v>13810.229699115</v>
+        <v>19505.013097345101</v>
       </c>
       <c r="AE34" s="7" t="s">
         <v>21</v>
@@ -2845,11 +2939,11 @@
       </c>
       <c r="BB34">
         <f t="shared" si="10"/>
-        <v>19505.013097345101</v>
+        <v>48762.532743362797</v>
       </c>
       <c r="BC34">
         <f t="shared" si="11"/>
-        <v>13810.229699115</v>
+        <v>19505.013097345101</v>
       </c>
       <c r="BD34">
         <f t="shared" si="12"/>
@@ -2871,7 +2965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="35" spans="20:62" ht="15">
       <c r="T35" s="9" t="s">
         <v>43</v>
       </c>
@@ -2885,7 +2979,7 @@
         <v>2017</v>
       </c>
       <c r="X35">
-        <v>20793.080000000002</v>
+        <v>51982.699999999997</v>
       </c>
       <c r="Z35" s="7" t="s">
         <v>21</v>
@@ -2898,7 +2992,7 @@
         <v>2020</v>
       </c>
       <c r="AC35">
-        <v>14722.226000000001</v>
+        <v>20793.080000000002</v>
       </c>
       <c r="AE35" s="7" t="s">
         <v>21</v>
@@ -2962,11 +3056,11 @@
       </c>
       <c r="BB35">
         <f t="shared" si="10"/>
-        <v>20793.080000000002</v>
+        <v>51982.699999999997</v>
       </c>
       <c r="BC35">
         <f t="shared" si="11"/>
-        <v>14722.226000000001</v>
+        <v>20793.080000000002</v>
       </c>
       <c r="BD35">
         <f t="shared" si="12"/>
@@ -2988,7 +3082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="36" spans="20:62" ht="15">
       <c r="T36" s="9" t="s">
         <v>45</v>
       </c>
@@ -3002,7 +3096,7 @@
         <v>2017</v>
       </c>
       <c r="X36">
-        <v>21530.351999999999</v>
+        <v>32295.527999999998</v>
       </c>
       <c r="Z36" s="7" t="s">
         <v>21</v>
@@ -3015,7 +3109,7 @@
         <v>2020</v>
       </c>
       <c r="AC36">
-        <v>17575</v>
+        <v>21530.351999999999</v>
       </c>
       <c r="AE36" s="7" t="s">
         <v>21</v>
@@ -3079,11 +3173,11 @@
       </c>
       <c r="BB36">
         <f t="shared" si="10"/>
-        <v>21530.351999999999</v>
+        <v>32295.527999999998</v>
       </c>
       <c r="BC36">
         <f t="shared" si="11"/>
-        <v>17575</v>
+        <v>21530.351999999999</v>
       </c>
       <c r="BD36">
         <f t="shared" si="12"/>
@@ -3105,7 +3199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="37" spans="20:62" ht="15">
       <c r="T37" s="9" t="s">
         <v>47</v>
       </c>
@@ -3207,7 +3301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:62" ht="23.25">
       <c r="B38" s="31" t="s">
         <v>114</v>
       </c>
@@ -3312,7 +3406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="39" spans="20:62" ht="15">
       <c r="T39" s="9" t="s">
         <v>51</v>
       </c>
@@ -3414,7 +3508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:62" ht="15">
       <c r="C40" s="10" t="s">
         <v>115</v>
       </c>
@@ -3537,7 +3631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:62" ht="15">
       <c r="C41" s="3" t="s">
         <v>8</v>
       </c>
@@ -3556,7 +3650,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J41" s="15">
-        <v>0.7</v>
+        <v>0.70</v>
       </c>
       <c r="K41" s="15">
         <v>0.75</v>
@@ -3665,7 +3759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:62" ht="15">
       <c r="C42" t="str">
         <f>C41</f>
         <v>cmach_e</v>
@@ -3682,13 +3776,13 @@
         <v>0.47058823529411764</v>
       </c>
       <c r="I42" s="15">
-        <v>0.5</v>
+        <v>0.50</v>
       </c>
       <c r="J42" s="15">
         <v>0.65</v>
       </c>
       <c r="K42" s="15">
-        <v>0.7</v>
+        <v>0.70</v>
       </c>
       <c r="L42" s="15">
         <v>0.75</v>
@@ -3794,7 +3888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:62" ht="15">
       <c r="C43" t="str">
         <f>C42</f>
         <v>cmach_e</v>
@@ -3811,16 +3905,16 @@
         <v>0.47058823529411764</v>
       </c>
       <c r="I43" s="15">
-        <v>0.5</v>
+        <v>0.50</v>
       </c>
       <c r="J43" s="15">
-        <v>0.6</v>
+        <v>0.60</v>
       </c>
       <c r="K43" s="15">
         <v>0.65</v>
       </c>
       <c r="L43" s="15">
-        <v>0.7</v>
+        <v>0.70</v>
       </c>
       <c r="T43" s="9" t="s">
         <v>59</v>
@@ -3923,7 +4017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:62" ht="15">
       <c r="C44" t="str">
         <f>C43</f>
         <v>cmach_e</v>
@@ -3940,7 +4034,7 @@
         <v>0.47058823529411764</v>
       </c>
       <c r="I44" s="5">
-        <f t="shared" ref="I44:L44" si="22">H44</f>
+        <f t="shared" si="22" ref="I44:L44">H44</f>
         <v>0.47058823529411764</v>
       </c>
       <c r="J44" s="5">
@@ -3984,7 +4078,7 @@
         <v>2020</v>
       </c>
       <c r="AC44">
-        <v>24484.621581831001</v>
+        <v>38195.713600000003</v>
       </c>
       <c r="AE44" s="7" t="s">
         <v>21</v>
@@ -4052,7 +4146,7 @@
       </c>
       <c r="BC44">
         <f t="shared" si="11"/>
-        <v>24484.621581831001</v>
+        <v>38195.713600000003</v>
       </c>
       <c r="BD44">
         <f t="shared" si="12"/>
@@ -4074,7 +4168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="45" spans="20:62" ht="15">
       <c r="T45" t="s">
         <v>63</v>
       </c>
@@ -4088,7 +4182,7 @@
         <v>2017</v>
       </c>
       <c r="X45">
-        <v>22625.8151929204</v>
+        <v>56564.537982300899</v>
       </c>
       <c r="Z45" s="7" t="s">
         <v>21</v>
@@ -4101,7 +4195,7 @@
         <v>2020</v>
       </c>
       <c r="AC45">
-        <v>16019.866450973501</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="AE45" s="7" t="s">
         <v>21</v>
@@ -4165,11 +4259,11 @@
       </c>
       <c r="BB45">
         <f t="shared" si="10"/>
-        <v>22625.8151929204</v>
+        <v>56564.537982300899</v>
       </c>
       <c r="BC45">
         <f t="shared" si="11"/>
-        <v>16019.866450973501</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="BD45">
         <f t="shared" si="12"/>
@@ -4191,7 +4285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="46" spans="20:62" ht="15">
       <c r="T46" t="s">
         <v>65</v>
       </c>
@@ -4205,7 +4299,7 @@
         <v>2017</v>
       </c>
       <c r="X46">
-        <v>22625.8151929204</v>
+        <v>56564.537982300899</v>
       </c>
       <c r="Z46" s="7" t="s">
         <v>21</v>
@@ -4218,7 +4312,7 @@
         <v>2020</v>
       </c>
       <c r="AC46">
-        <v>16019.866450973501</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="AE46" s="7" t="s">
         <v>21</v>
@@ -4282,11 +4376,11 @@
       </c>
       <c r="BB46">
         <f t="shared" si="10"/>
-        <v>22625.8151929204</v>
+        <v>56564.537982300899</v>
       </c>
       <c r="BC46">
         <f t="shared" si="11"/>
-        <v>16019.866450973501</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="BD46">
         <f t="shared" si="12"/>
@@ -4308,7 +4402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:62" ht="15">
       <c r="C47" s="10" t="s">
         <v>116</v>
       </c>
@@ -4325,7 +4419,7 @@
         <v>2017</v>
       </c>
       <c r="X47">
-        <v>22625.8151929204</v>
+        <v>56564.537982300899</v>
       </c>
       <c r="Z47" s="7" t="s">
         <v>21</v>
@@ -4338,7 +4432,7 @@
         <v>2020</v>
       </c>
       <c r="AC47">
-        <v>16019.866450973501</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="AE47" s="7" t="s">
         <v>21</v>
@@ -4402,11 +4496,11 @@
       </c>
       <c r="BB47">
         <f t="shared" si="10"/>
-        <v>22625.8151929204</v>
+        <v>56564.537982300899</v>
       </c>
       <c r="BC47">
         <f t="shared" si="11"/>
-        <v>16019.866450973501</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="BD47">
         <f t="shared" si="12"/>
@@ -4428,7 +4522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:62" ht="15">
       <c r="C48" s="3" t="s">
         <v>11</v>
       </c>
@@ -4447,7 +4541,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J48" s="15">
-        <v>0.7</v>
+        <v>0.70</v>
       </c>
       <c r="K48" s="15">
         <v>0.75</v>
@@ -4468,7 +4562,7 @@
         <v>2017</v>
       </c>
       <c r="X48">
-        <v>34133.772920354</v>
+        <v>85334.432300885004</v>
       </c>
       <c r="Z48" s="7" t="s">
         <v>21</v>
@@ -4481,7 +4575,7 @@
         <v>2020</v>
       </c>
       <c r="AC48">
-        <v>24167.901973451299</v>
+        <v>34133.772920354</v>
       </c>
       <c r="AE48" s="7" t="s">
         <v>21</v>
@@ -4545,11 +4639,11 @@
       </c>
       <c r="BB48">
         <f t="shared" si="10"/>
-        <v>34133.772920354</v>
+        <v>85334.432300885004</v>
       </c>
       <c r="BC48">
         <f t="shared" si="11"/>
-        <v>24167.901973451299</v>
+        <v>34133.772920354</v>
       </c>
       <c r="BD48">
         <f t="shared" si="12"/>
@@ -4571,7 +4665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:62" ht="15">
       <c r="C49" t="str">
         <f>C48</f>
         <v>cemch_e</v>
@@ -4588,13 +4682,13 @@
         <v>0.47538200339558578</v>
       </c>
       <c r="I49" s="15">
-        <v>0.5</v>
+        <v>0.50</v>
       </c>
       <c r="J49" s="15">
         <v>0.65</v>
       </c>
       <c r="K49" s="15">
-        <v>0.7</v>
+        <v>0.70</v>
       </c>
       <c r="L49" s="15">
         <v>0.75</v>
@@ -4612,7 +4706,7 @@
         <v>2017</v>
       </c>
       <c r="X49">
-        <v>22625.8151929204</v>
+        <v>56564.537982300899</v>
       </c>
       <c r="Z49" s="7" t="s">
         <v>21</v>
@@ -4625,7 +4719,7 @@
         <v>2020</v>
       </c>
       <c r="AC49">
-        <v>16019.866450973501</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="AE49" s="7" t="s">
         <v>21</v>
@@ -4689,11 +4783,11 @@
       </c>
       <c r="BB49">
         <f t="shared" si="10"/>
-        <v>22625.8151929204</v>
+        <v>56564.537982300899</v>
       </c>
       <c r="BC49">
         <f t="shared" si="11"/>
-        <v>16019.866450973501</v>
+        <v>22625.8151929204</v>
       </c>
       <c r="BD49">
         <f t="shared" si="12"/>
@@ -4715,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:62" ht="15">
       <c r="C50" t="str">
         <f>C49</f>
         <v>cemch_e</v>
@@ -4732,16 +4826,16 @@
         <v>0.47538200339558578</v>
       </c>
       <c r="I50" s="15">
-        <v>0.5</v>
+        <v>0.50</v>
       </c>
       <c r="J50" s="15">
-        <v>0.6</v>
+        <v>0.60</v>
       </c>
       <c r="K50" s="15">
         <v>0.65</v>
       </c>
       <c r="L50" s="15">
-        <v>0.7</v>
+        <v>0.70</v>
       </c>
       <c r="T50" s="9" t="s">
         <v>73</v>
@@ -4756,7 +4850,7 @@
         <v>2017</v>
       </c>
       <c r="X50">
-        <v>6329.3065449900196</v>
+        <v>1637.60737116</v>
       </c>
       <c r="Z50" s="7"/>
       <c r="AA50" s="9"/>
@@ -4780,13 +4874,13 @@
       </c>
       <c r="BB50">
         <f t="shared" si="10"/>
-        <v>6329.3065449900196</v>
+        <v>1637.60737116</v>
       </c>
       <c r="BJ50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:28 47:62" ht="15">
       <c r="C51" t="str">
         <f>C50</f>
         <v>cemch_e</v>
@@ -4803,7 +4897,7 @@
         <v>0.47538200339558578</v>
       </c>
       <c r="I51" s="5">
-        <f t="shared" ref="I51:L51" si="23">H51</f>
+        <f t="shared" si="23" ref="I51:L51">H51</f>
         <v>0.47538200339558578</v>
       </c>
       <c r="J51" s="5">
@@ -4834,7 +4928,7 @@
         <v>2017</v>
       </c>
       <c r="X51">
-        <v>2812</v>
+        <v>337.44</v>
       </c>
       <c r="Z51" s="7"/>
       <c r="AA51" s="9"/>
@@ -4852,13 +4946,13 @@
       </c>
       <c r="BB51">
         <f t="shared" si="10"/>
-        <v>2812</v>
+        <v>337.44</v>
       </c>
       <c r="BJ51">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="52" spans="20:62" ht="15">
       <c r="T52" s="9" t="s">
         <v>77</v>
       </c>
@@ -4872,7 +4966,7 @@
         <v>2017</v>
       </c>
       <c r="X52">
-        <v>36989.331580508697</v>
+        <v>19046.524215158599</v>
       </c>
       <c r="Z52" s="7"/>
       <c r="AA52" s="9"/>
@@ -4890,13 +4984,13 @@
       </c>
       <c r="BB52">
         <f t="shared" si="10"/>
-        <v>36989.331580508697</v>
+        <v>19046.524215158599</v>
       </c>
       <c r="BJ52">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3 20:28 47:62" ht="15">
       <c r="C53" s="10" t="s">
         <v>117</v>
       </c>
@@ -4913,7 +5007,7 @@
         <v>2017</v>
       </c>
       <c r="X53">
-        <v>18494.665850167301</v>
+        <v>9523.2621384296508</v>
       </c>
       <c r="Z53" s="7"/>
       <c r="AA53" s="9"/>
@@ -4931,13 +5025,13 @@
       </c>
       <c r="BB53">
         <f t="shared" si="10"/>
-        <v>18494.665850167301</v>
+        <v>9523.2621384296508</v>
       </c>
       <c r="BJ53">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:28 47:62" ht="15">
       <c r="C54" t="s">
         <v>128</v>
       </c>
@@ -4949,7 +5043,7 @@
         <v>0.93842364532019706</v>
       </c>
       <c r="H54" s="6">
-        <f t="shared" ref="H54:I56" si="24">G54</f>
+        <f t="shared" si="24" ref="H54:I56">G54</f>
         <v>0.93842364532019706</v>
       </c>
       <c r="I54" s="15">
@@ -4961,16 +5055,16 @@
         <v>0.94827586206896552</v>
       </c>
       <c r="K54" s="15">
-        <f t="shared" ref="K54:K55" si="25">J54</f>
+        <f t="shared" si="25" ref="K54:K55">J54</f>
         <v>0.94827586206896552</v>
       </c>
       <c r="L54" s="15">
-        <f t="shared" ref="L54:L55" si="26">K54</f>
+        <f t="shared" si="26" ref="L54:L55">K54</f>
         <v>0.94827586206896552</v>
       </c>
       <c r="O54" s="5">
         <f>J81</f>
-        <v>9.852216748768473E-3</v>
+        <v>0.009852216748768473</v>
       </c>
       <c r="T54" s="9" t="s">
         <v>81</v>
@@ -4985,7 +5079,7 @@
         <v>2017</v>
       </c>
       <c r="X54">
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="Z54" s="7"/>
       <c r="AA54" s="9"/>
@@ -5003,13 +5097,13 @@
       </c>
       <c r="BB54">
         <f t="shared" si="10"/>
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="BJ54">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:28 47:62" ht="15">
       <c r="C55" t="s">
         <v>128</v>
       </c>
@@ -5053,7 +5147,7 @@
         <v>2017</v>
       </c>
       <c r="X55">
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="Z55" s="7"/>
       <c r="AA55" s="9"/>
@@ -5071,13 +5165,13 @@
       </c>
       <c r="BB55">
         <f t="shared" si="10"/>
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="BJ55">
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:28 47:62" ht="15">
       <c r="C56" t="s">
         <v>128</v>
       </c>
@@ -5120,7 +5214,7 @@
         <v>2017</v>
       </c>
       <c r="X56">
-        <v>14124.4235169599</v>
+        <v>7272.9396030149201</v>
       </c>
       <c r="Z56" s="7"/>
       <c r="AA56" s="9"/>
@@ -5138,13 +5232,13 @@
       </c>
       <c r="BB56">
         <f t="shared" si="10"/>
-        <v>14124.4235169599</v>
+        <v>7272.9396030149201</v>
       </c>
       <c r="BJ56">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:24 52:62" ht="15">
       <c r="C57" t="s">
         <v>128</v>
       </c>
@@ -5168,7 +5262,7 @@
         <v>0.93842364532019706</v>
       </c>
       <c r="K57" s="6">
-        <f t="shared" ref="K57:L57" si="27">J57</f>
+        <f t="shared" si="27" ref="K57:L57">J57</f>
         <v>0.93842364532019706</v>
       </c>
       <c r="L57" s="6">
@@ -5191,7 +5285,7 @@
         <v>2017</v>
       </c>
       <c r="X57">
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="AZ57" t="str">
         <f t="shared" si="20"/>
@@ -5203,13 +5297,13 @@
       </c>
       <c r="BB57">
         <f t="shared" si="10"/>
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="BJ57">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="58" spans="20:24 52:62" ht="15">
       <c r="T58" s="9" t="s">
         <v>89</v>
       </c>
@@ -5223,7 +5317,7 @@
         <v>2017</v>
       </c>
       <c r="X58">
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="AZ58" t="str">
         <f t="shared" si="20"/>
@@ -5235,13 +5329,13 @@
       </c>
       <c r="BB58">
         <f t="shared" si="10"/>
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="BJ58">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3 20:24 52:62" ht="15">
       <c r="C59" s="10" t="s">
         <v>118</v>
       </c>
@@ -5258,7 +5352,7 @@
         <v>2017</v>
       </c>
       <c r="X59">
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="AZ59" t="str">
         <f t="shared" si="20"/>
@@ -5270,13 +5364,13 @@
       </c>
       <c r="BB59">
         <f t="shared" si="10"/>
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="BJ59">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:24 52:62" ht="15">
       <c r="C60" s="3" t="s">
         <v>123</v>
       </c>
@@ -5288,7 +5382,7 @@
         <v>0.76065573770491801</v>
       </c>
       <c r="H60" s="6">
-        <f t="shared" ref="H60:I62" si="28">G60</f>
+        <f t="shared" si="28" ref="H60:I62">G60</f>
         <v>0.76065573770491801</v>
       </c>
       <c r="I60" s="15">
@@ -5300,7 +5394,7 @@
         <v>0.78098360655737697</v>
       </c>
       <c r="K60" s="15">
-        <f t="shared" ref="K60:L63" si="29">J60</f>
+        <f t="shared" si="29" ref="K60:L63">J60</f>
         <v>0.78098360655737697</v>
       </c>
       <c r="L60" s="15">
@@ -5309,7 +5403,7 @@
       </c>
       <c r="O60" s="28">
         <f>J83</f>
-        <v>2.0327868852459016E-2</v>
+        <v>0.020327868852459016</v>
       </c>
       <c r="T60" s="9" t="s">
         <v>93</v>
@@ -5324,7 +5418,7 @@
         <v>2017</v>
       </c>
       <c r="X60">
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="AZ60" t="str">
         <f t="shared" si="20"/>
@@ -5336,13 +5430,13 @@
       </c>
       <c r="BB60">
         <f t="shared" si="10"/>
-        <v>8791.3381114607892</v>
+        <v>4526.8304959535499</v>
       </c>
       <c r="BJ60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:24 52:62" ht="15">
       <c r="C61" t="str">
         <f>C60</f>
         <v>cmetp</v>
@@ -5387,7 +5481,7 @@
         <v>2017</v>
       </c>
       <c r="X61">
-        <v>14124.4235169599</v>
+        <v>7272.9396030149201</v>
       </c>
       <c r="AZ61" t="str">
         <f t="shared" si="20"/>
@@ -5399,13 +5493,13 @@
       </c>
       <c r="BB61">
         <f t="shared" si="10"/>
-        <v>14124.4235169599</v>
+        <v>7272.9396030149201</v>
       </c>
       <c r="BJ61">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:24 52:62" ht="15">
       <c r="C62" t="str">
         <f>C61</f>
         <v>cmetp</v>
@@ -5450,7 +5544,7 @@
         <v>2017</v>
       </c>
       <c r="X62">
-        <v>14124.4235169599</v>
+        <v>7272.9396030149201</v>
       </c>
       <c r="AZ62" t="str">
         <f t="shared" si="20"/>
@@ -5462,13 +5556,13 @@
       </c>
       <c r="BB62">
         <f t="shared" si="10"/>
-        <v>14124.4235169599</v>
+        <v>7272.9396030149201</v>
       </c>
       <c r="BJ62">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:24 52:62" ht="15">
       <c r="C63" t="str">
         <f>C62</f>
         <v>cmetp</v>
@@ -5489,7 +5583,7 @@
         <v>0.76065573770491801</v>
       </c>
       <c r="J63" s="6">
-        <f t="shared" ref="J63" si="30">I63</f>
+        <f t="shared" si="30" ref="J63">I63</f>
         <v>0.76065573770491801</v>
       </c>
       <c r="K63" s="6">
@@ -5516,7 +5610,7 @@
         <v>2017</v>
       </c>
       <c r="X63">
-        <v>36989.331580508697</v>
+        <v>19046.524215158599</v>
       </c>
       <c r="AZ63" t="str">
         <f t="shared" si="20"/>
@@ -5528,13 +5622,13 @@
       </c>
       <c r="BB63">
         <f t="shared" si="10"/>
-        <v>36989.331580508697</v>
+        <v>19046.524215158599</v>
       </c>
       <c r="BJ63">
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="3:62" x14ac:dyDescent="0.25">
+    <row r="64" spans="20:24 52:62" ht="15">
       <c r="T64" s="9" t="s">
         <v>101</v>
       </c>
@@ -5548,7 +5642,7 @@
         <v>2017</v>
       </c>
       <c r="X64">
-        <v>18494.665850167301</v>
+        <v>9523.2621384296508</v>
       </c>
       <c r="AZ64" t="str">
         <f t="shared" si="20"/>
@@ -5560,13 +5654,13 @@
       </c>
       <c r="BB64">
         <f t="shared" si="10"/>
-        <v>18494.665850167301</v>
+        <v>9523.2621384296508</v>
       </c>
       <c r="BJ64">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="2:62" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:2 20:24 52:62" ht="23.25">
       <c r="B65" s="31" t="s">
         <v>134</v>
       </c>
@@ -5583,7 +5677,7 @@
         <v>2017</v>
       </c>
       <c r="X65">
-        <v>9247.3329250836705</v>
+        <v>4761.6310692148199</v>
       </c>
       <c r="AZ65" t="str">
         <f t="shared" si="20"/>
@@ -5595,13 +5689,13 @@
       </c>
       <c r="BB65">
         <f t="shared" si="10"/>
-        <v>9247.3329250836705</v>
+        <v>4761.6310692148199</v>
       </c>
       <c r="BJ65">
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:23" ht="15">
       <c r="F66" t="s">
         <v>111</v>
       </c>
@@ -5621,12 +5715,12 @@
         <v>0.125</v>
       </c>
       <c r="L66" s="6">
-        <v>0.2</v>
+        <v>0.20</v>
       </c>
       <c r="V66" s="9"/>
       <c r="W66" s="9"/>
     </row>
-    <row r="67" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:12" ht="15">
       <c r="F67" t="s">
         <v>112</v>
       </c>
@@ -5643,13 +5737,13 @@
         <v>0.05</v>
       </c>
       <c r="K67" s="6">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="L67" s="6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="68" spans="2:62" x14ac:dyDescent="0.25">
+        <v>0.10</v>
+      </c>
+    </row>
+    <row r="68" spans="6:12" ht="15">
       <c r="F68" t="s">
         <v>113</v>
       </c>
@@ -5663,18 +5757,18 @@
         <v>0.01</v>
       </c>
       <c r="J68" s="5">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="K68" s="5">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="L68" s="5">
         <v>0.05</v>
       </c>
     </row>
-    <row r="69" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:12" ht="15">
       <c r="F69" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G69" s="6">
         <v>0</v>
@@ -5695,7 +5789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="79" spans="7:11" ht="15">
       <c r="G79" t="s">
         <v>129</v>
       </c>
@@ -5712,7 +5806,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="80" spans="2:62" x14ac:dyDescent="0.25">
+    <row r="80" spans="6:10" ht="15">
       <c r="F80" t="s">
         <v>128</v>
       </c>
@@ -5730,22 +5824,22 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="7:10" ht="15">
       <c r="G81" s="4">
         <f>G80/I80</f>
-        <v>6.1576354679802957E-2</v>
+        <v>0.061576354679802957</v>
       </c>
       <c r="J81" s="29">
         <f>J80/I80</f>
-        <v>9.852216748768473E-3</v>
-      </c>
-    </row>
-    <row r="82" spans="6:10" x14ac:dyDescent="0.25">
+        <v>0.009852216748768473</v>
+      </c>
+    </row>
+    <row r="82" spans="6:10" ht="15">
       <c r="F82" t="s">
         <v>133</v>
       </c>
       <c r="G82">
-        <v>36.5</v>
+        <v>36.50</v>
       </c>
       <c r="H82">
         <v>116</v>
@@ -5755,30 +5849,30 @@
         <v>152.5</v>
       </c>
       <c r="J82">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="83" spans="6:10" x14ac:dyDescent="0.25">
+        <v>3.10</v>
+      </c>
+    </row>
+    <row r="83" spans="7:10" ht="15">
       <c r="G83" s="29">
         <f>G82/I82</f>
         <v>0.23934426229508196</v>
       </c>
       <c r="J83" s="29">
         <f>J82/I82</f>
-        <v>2.0327868852459016E-2</v>
+        <v>0.020327868852459016</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{28F83205-2B6D-4B86-9C9B-CC3DB94DE282}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
       <formula1>$F$41:$F$44</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{B1584D95-3338-4846-9756-AAD3A2F15D0C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
       <formula1>$F$66:$F$69</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>